<commit_message>
Add new moisture data file for cracking team experiment and update large batch data
</commit_message>
<xml_diff>
--- a/moisture-team-data/largebatch/large.xlsx
+++ b/moisture-team-data/largebatch/large.xlsx
@@ -4,7 +4,7 @@
   <fileVersion rupBuild="9303" lowestEdited="5" lastEdited="5" appName="xl"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="0"/>
+    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet r:id="rId1" sheetId="1" name="Pilot Study"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="576" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="577" uniqueCount="48">
   <si>
     <t>Sample 1</t>
   </si>
@@ -97,6 +97,9 @@
     <t>31 hours of cold soaking</t>
   </si>
   <si>
+    <t>horizontal</t>
+  </si>
+  <si>
     <t>14 hours of cold soaking</t>
   </si>
   <si>
@@ -165,7 +168,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
   <numFmts count="0"/>
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -188,20 +191,14 @@
     </font>
     <font>
       <sz val="12"/>
-      <color theme="1"/>
-      <name val="Times New Roman"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Times New Roman"/>
       <family val="2"/>
     </font>
     <font>
-      <sz val="15"/>
+      <sz val="11"/>
       <color theme="1"/>
-      <name val="Times New Roman"/>
+      <name val="Calibri"/>
       <family val="2"/>
     </font>
     <font>
@@ -225,7 +222,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -588,7 +585,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="107">
+  <cellXfs count="105">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -677,9 +674,6 @@
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf xfId="0" numFmtId="0" borderId="12" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -713,11 +707,14 @@
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -794,11 +791,14 @@
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="10" applyBorder="1" fontId="1" applyFont="1" fillId="4" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="16" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -836,10 +836,7 @@
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="5" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="6" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="6" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="5" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="18" applyBorder="1" fontId="1" applyFont="1" fillId="4" applyFill="1" applyAlignment="1">
@@ -848,7 +845,7 @@
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="18" applyBorder="1" fontId="1" applyFont="1" fillId="4" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="6" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="5" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="19" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
@@ -857,13 +854,7 @@
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="19" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="7" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="5" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="5" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="6" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
@@ -896,16 +887,16 @@
     <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="20" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="24" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="24" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="25" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="20" applyBorder="1" fontId="8" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="20" applyBorder="1" fontId="7" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="9" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="8" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1212,35 +1203,35 @@
   </sheetPr>
   <dimension ref="A1:Y12"/>
   <sheetViews>
-    <sheetView workbookViewId="0" tabSelected="1"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="41" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="41" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="41" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="41" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="39" width="20.719285714285714" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="40" width="20.719285714285714" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="40" width="20.719285714285714" customWidth="1" bestFit="1"/>
-    <col min="8" max="8" style="40" width="20.719285714285714" customWidth="1" bestFit="1"/>
-    <col min="9" max="9" style="39" width="20.719285714285714" customWidth="1" bestFit="1"/>
-    <col min="10" max="10" style="40" width="20.719285714285714" customWidth="1" bestFit="1"/>
-    <col min="11" max="11" style="40" width="20.719285714285714" customWidth="1" bestFit="1"/>
-    <col min="12" max="12" style="40" width="20.719285714285714" customWidth="1" bestFit="1"/>
-    <col min="13" max="13" style="40" width="20.719285714285714" customWidth="1" bestFit="1"/>
-    <col min="14" max="14" style="41" width="20.719285714285714" customWidth="1" bestFit="1"/>
-    <col min="15" max="15" style="39" width="20.719285714285714" customWidth="1" bestFit="1"/>
-    <col min="16" max="16" style="39" width="20.719285714285714" customWidth="1" bestFit="1"/>
-    <col min="17" max="17" style="40" width="20.719285714285714" customWidth="1" bestFit="1"/>
-    <col min="18" max="18" style="40" width="20.719285714285714" customWidth="1" bestFit="1"/>
-    <col min="19" max="19" style="39" width="20.719285714285714" customWidth="1" bestFit="1"/>
-    <col min="20" max="20" style="40" width="20.719285714285714" customWidth="1" bestFit="1"/>
-    <col min="21" max="21" style="40" width="20.719285714285714" customWidth="1" bestFit="1"/>
-    <col min="22" max="22" style="40" width="20.719285714285714" customWidth="1" bestFit="1"/>
-    <col min="23" max="23" style="40" width="20.719285714285714" customWidth="1" bestFit="1"/>
-    <col min="24" max="24" style="40" width="20.719285714285714" customWidth="1" bestFit="1"/>
-    <col min="25" max="25" style="40" width="20.719285714285714" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="40" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="40" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="40" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="40" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="38" width="20.719285714285714" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="39" width="20.719285714285714" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="38" width="20.719285714285714" customWidth="1" bestFit="1"/>
+    <col min="8" max="8" style="39" width="20.719285714285714" customWidth="1" bestFit="1"/>
+    <col min="9" max="9" style="38" width="20.719285714285714" customWidth="1" bestFit="1"/>
+    <col min="10" max="10" style="39" width="20.719285714285714" customWidth="1" bestFit="1"/>
+    <col min="11" max="11" style="38" width="20.719285714285714" customWidth="1" bestFit="1"/>
+    <col min="12" max="12" style="39" width="20.719285714285714" customWidth="1" bestFit="1"/>
+    <col min="13" max="13" style="39" width="20.719285714285714" customWidth="1" bestFit="1"/>
+    <col min="14" max="14" style="40" width="20.719285714285714" customWidth="1" bestFit="1"/>
+    <col min="15" max="15" style="38" width="20.719285714285714" customWidth="1" bestFit="1"/>
+    <col min="16" max="16" style="38" width="20.719285714285714" customWidth="1" bestFit="1"/>
+    <col min="17" max="17" style="38" width="20.719285714285714" customWidth="1" bestFit="1"/>
+    <col min="18" max="18" style="39" width="20.719285714285714" customWidth="1" bestFit="1"/>
+    <col min="19" max="19" style="38" width="20.719285714285714" customWidth="1" bestFit="1"/>
+    <col min="20" max="20" style="39" width="20.719285714285714" customWidth="1" bestFit="1"/>
+    <col min="21" max="21" style="38" width="20.719285714285714" customWidth="1" bestFit="1"/>
+    <col min="22" max="22" style="39" width="20.719285714285714" customWidth="1" bestFit="1"/>
+    <col min="23" max="23" style="38" width="20.719285714285714" customWidth="1" bestFit="1"/>
+    <col min="24" max="24" style="39" width="20.719285714285714" customWidth="1" bestFit="1"/>
+    <col min="25" max="25" style="39" width="20.719285714285714" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
@@ -1248,604 +1239,604 @@
       <c r="B1" s="4"/>
       <c r="C1" s="4"/>
       <c r="D1" s="4"/>
-      <c r="E1" s="42"/>
-      <c r="F1" s="43"/>
-      <c r="G1" s="43"/>
-      <c r="H1" s="43"/>
-      <c r="I1" s="42"/>
-      <c r="J1" s="43"/>
-      <c r="K1" s="43"/>
-      <c r="L1" s="43"/>
-      <c r="M1" s="43"/>
+      <c r="E1" s="41"/>
+      <c r="F1" s="42"/>
+      <c r="G1" s="42"/>
+      <c r="H1" s="42"/>
+      <c r="I1" s="41"/>
+      <c r="J1" s="42"/>
+      <c r="K1" s="42"/>
+      <c r="L1" s="42"/>
+      <c r="M1" s="42"/>
       <c r="N1" s="4"/>
-      <c r="O1" s="42"/>
-      <c r="P1" s="42"/>
-      <c r="Q1" s="43"/>
-      <c r="R1" s="43"/>
-      <c r="S1" s="42"/>
-      <c r="T1" s="43"/>
-      <c r="U1" s="43"/>
-      <c r="V1" s="43"/>
-      <c r="W1" s="43"/>
-      <c r="X1" s="43"/>
-      <c r="Y1" s="43"/>
+      <c r="O1" s="41"/>
+      <c r="P1" s="41"/>
+      <c r="Q1" s="42"/>
+      <c r="R1" s="42"/>
+      <c r="S1" s="41"/>
+      <c r="T1" s="42"/>
+      <c r="U1" s="42"/>
+      <c r="V1" s="42"/>
+      <c r="W1" s="42"/>
+      <c r="X1" s="42"/>
+      <c r="Y1" s="42"/>
     </row>
     <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
       <c r="A2" s="4"/>
       <c r="B2" s="4"/>
       <c r="C2" s="4"/>
       <c r="D2" s="4"/>
-      <c r="E2" s="42"/>
-      <c r="F2" s="43"/>
-      <c r="G2" s="43"/>
-      <c r="H2" s="43"/>
-      <c r="I2" s="42"/>
-      <c r="J2" s="43"/>
-      <c r="K2" s="43"/>
-      <c r="L2" s="43"/>
-      <c r="M2" s="43"/>
+      <c r="E2" s="41"/>
+      <c r="F2" s="42"/>
+      <c r="G2" s="42"/>
+      <c r="H2" s="42"/>
+      <c r="I2" s="41"/>
+      <c r="J2" s="42"/>
+      <c r="K2" s="42"/>
+      <c r="L2" s="42"/>
+      <c r="M2" s="42"/>
       <c r="N2" s="4"/>
-      <c r="O2" s="42"/>
-      <c r="P2" s="42"/>
-      <c r="Q2" s="43"/>
-      <c r="R2" s="43"/>
-      <c r="S2" s="42"/>
-      <c r="T2" s="43"/>
-      <c r="U2" s="43"/>
-      <c r="V2" s="43"/>
-      <c r="W2" s="43"/>
-      <c r="X2" s="43"/>
-      <c r="Y2" s="43"/>
+      <c r="O2" s="41"/>
+      <c r="P2" s="41"/>
+      <c r="Q2" s="42"/>
+      <c r="R2" s="42"/>
+      <c r="S2" s="41"/>
+      <c r="T2" s="42"/>
+      <c r="U2" s="42"/>
+      <c r="V2" s="42"/>
+      <c r="W2" s="42"/>
+      <c r="X2" s="42"/>
+      <c r="Y2" s="42"/>
     </row>
     <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
       <c r="A3" s="4"/>
       <c r="B3" s="4"/>
       <c r="C3" s="4"/>
       <c r="D3" s="4"/>
-      <c r="E3" s="42"/>
-      <c r="F3" s="43"/>
-      <c r="G3" s="43"/>
-      <c r="H3" s="43"/>
-      <c r="I3" s="42"/>
-      <c r="J3" s="43"/>
-      <c r="K3" s="43"/>
-      <c r="L3" s="43"/>
-      <c r="M3" s="43"/>
+      <c r="E3" s="41"/>
+      <c r="F3" s="42"/>
+      <c r="G3" s="42"/>
+      <c r="H3" s="42"/>
+      <c r="I3" s="41"/>
+      <c r="J3" s="42"/>
+      <c r="K3" s="42"/>
+      <c r="L3" s="42"/>
+      <c r="M3" s="42"/>
       <c r="N3" s="4"/>
-      <c r="O3" s="42"/>
-      <c r="P3" s="42"/>
-      <c r="Q3" s="43"/>
-      <c r="R3" s="43"/>
-      <c r="S3" s="42"/>
-      <c r="T3" s="43"/>
-      <c r="U3" s="43"/>
-      <c r="V3" s="43"/>
-      <c r="W3" s="43"/>
-      <c r="X3" s="43"/>
-      <c r="Y3" s="43"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
+      <c r="O3" s="41"/>
+      <c r="P3" s="41"/>
+      <c r="Q3" s="42"/>
+      <c r="R3" s="42"/>
+      <c r="S3" s="41"/>
+      <c r="T3" s="42"/>
+      <c r="U3" s="42"/>
+      <c r="V3" s="42"/>
+      <c r="W3" s="42"/>
+      <c r="X3" s="42"/>
+      <c r="Y3" s="42"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="23.25">
       <c r="A4" s="4"/>
       <c r="B4" s="4"/>
       <c r="C4" s="4"/>
       <c r="D4" s="4"/>
-      <c r="E4" s="95" t="s">
-        <v>38</v>
-      </c>
-      <c r="F4" s="96"/>
-      <c r="G4" s="96"/>
-      <c r="H4" s="96"/>
-      <c r="I4" s="95"/>
-      <c r="J4" s="96"/>
-      <c r="K4" s="96"/>
-      <c r="L4" s="96"/>
-      <c r="M4" s="96"/>
+      <c r="E4" s="93" t="s">
+        <v>39</v>
+      </c>
+      <c r="F4" s="94"/>
+      <c r="G4" s="94"/>
+      <c r="H4" s="94"/>
+      <c r="I4" s="93"/>
+      <c r="J4" s="94"/>
+      <c r="K4" s="94"/>
+      <c r="L4" s="94"/>
+      <c r="M4" s="94"/>
       <c r="N4" s="4"/>
-      <c r="O4" s="97" t="s">
-        <v>39</v>
-      </c>
-      <c r="P4" s="98"/>
-      <c r="Q4" s="99"/>
-      <c r="R4" s="99"/>
-      <c r="S4" s="98"/>
-      <c r="T4" s="99"/>
-      <c r="U4" s="99"/>
-      <c r="V4" s="99"/>
-      <c r="W4" s="99"/>
-      <c r="X4" s="99"/>
-      <c r="Y4" s="100"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
+      <c r="O4" s="95" t="s">
+        <v>40</v>
+      </c>
+      <c r="P4" s="96"/>
+      <c r="Q4" s="97"/>
+      <c r="R4" s="97"/>
+      <c r="S4" s="96"/>
+      <c r="T4" s="97"/>
+      <c r="U4" s="97"/>
+      <c r="V4" s="97"/>
+      <c r="W4" s="97"/>
+      <c r="X4" s="97"/>
+      <c r="Y4" s="98"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="23.25">
       <c r="A5" s="4"/>
       <c r="B5" s="4"/>
       <c r="C5" s="4"/>
       <c r="D5" s="4"/>
-      <c r="E5" s="101" t="s">
-        <v>40</v>
-      </c>
-      <c r="F5" s="102"/>
-      <c r="G5" s="102" t="s">
+      <c r="E5" s="99" t="s">
         <v>41</v>
       </c>
-      <c r="H5" s="102"/>
-      <c r="I5" s="101" t="s">
+      <c r="F5" s="100"/>
+      <c r="G5" s="99" t="s">
         <v>42</v>
       </c>
-      <c r="J5" s="102"/>
-      <c r="K5" s="102" t="s">
+      <c r="H5" s="100"/>
+      <c r="I5" s="99" t="s">
         <v>43</v>
       </c>
-      <c r="L5" s="102"/>
-      <c r="M5" s="102" t="s">
+      <c r="J5" s="100"/>
+      <c r="K5" s="99" t="s">
         <v>44</v>
       </c>
+      <c r="L5" s="100"/>
+      <c r="M5" s="100" t="s">
+        <v>45</v>
+      </c>
       <c r="N5" s="4"/>
-      <c r="O5" s="101" t="s">
+      <c r="O5" s="99" t="s">
         <v>0</v>
       </c>
-      <c r="P5" s="101"/>
-      <c r="Q5" s="102" t="s">
+      <c r="P5" s="99"/>
+      <c r="Q5" s="99" t="s">
         <v>1</v>
       </c>
-      <c r="R5" s="102"/>
-      <c r="S5" s="101" t="s">
+      <c r="R5" s="100"/>
+      <c r="S5" s="99" t="s">
         <v>2</v>
       </c>
-      <c r="T5" s="102"/>
-      <c r="U5" s="102" t="s">
+      <c r="T5" s="100"/>
+      <c r="U5" s="99" t="s">
         <v>3</v>
       </c>
-      <c r="V5" s="102"/>
-      <c r="W5" s="103" t="s">
+      <c r="V5" s="100"/>
+      <c r="W5" s="101" t="s">
         <v>4</v>
       </c>
-      <c r="X5" s="104"/>
-      <c r="Y5" s="102" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
+      <c r="X5" s="102"/>
+      <c r="Y5" s="100" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="23.25">
       <c r="A6" s="4"/>
       <c r="B6" s="4"/>
       <c r="C6" s="4"/>
       <c r="D6" s="4"/>
-      <c r="E6" s="101" t="s">
-        <v>45</v>
-      </c>
-      <c r="F6" s="102" t="s">
+      <c r="E6" s="99" t="s">
         <v>46</v>
       </c>
-      <c r="G6" s="102" t="s">
-        <v>45</v>
-      </c>
-      <c r="H6" s="102" t="s">
+      <c r="F6" s="100" t="s">
+        <v>47</v>
+      </c>
+      <c r="G6" s="99" t="s">
         <v>46</v>
       </c>
-      <c r="I6" s="101" t="s">
-        <v>45</v>
-      </c>
-      <c r="J6" s="102" t="s">
+      <c r="H6" s="100" t="s">
+        <v>47</v>
+      </c>
+      <c r="I6" s="99" t="s">
         <v>46</v>
       </c>
-      <c r="K6" s="102" t="s">
-        <v>45</v>
-      </c>
-      <c r="L6" s="102" t="s">
+      <c r="J6" s="100" t="s">
+        <v>47</v>
+      </c>
+      <c r="K6" s="99" t="s">
         <v>46</v>
       </c>
-      <c r="M6" s="105"/>
-      <c r="N6" s="106"/>
-      <c r="O6" s="101" t="s">
-        <v>45</v>
-      </c>
-      <c r="P6" s="101" t="s">
+      <c r="L6" s="100" t="s">
+        <v>47</v>
+      </c>
+      <c r="M6" s="103"/>
+      <c r="N6" s="104"/>
+      <c r="O6" s="99" t="s">
         <v>46</v>
       </c>
-      <c r="Q6" s="102" t="s">
-        <v>45</v>
-      </c>
-      <c r="R6" s="102" t="s">
+      <c r="P6" s="99" t="s">
+        <v>47</v>
+      </c>
+      <c r="Q6" s="99" t="s">
         <v>46</v>
       </c>
-      <c r="S6" s="101" t="s">
-        <v>45</v>
-      </c>
-      <c r="T6" s="102" t="s">
+      <c r="R6" s="100" t="s">
+        <v>47</v>
+      </c>
+      <c r="S6" s="99" t="s">
         <v>46</v>
       </c>
-      <c r="U6" s="102" t="s">
-        <v>45</v>
-      </c>
-      <c r="V6" s="102" t="s">
+      <c r="T6" s="100" t="s">
+        <v>47</v>
+      </c>
+      <c r="U6" s="99" t="s">
         <v>46</v>
       </c>
-      <c r="W6" s="102" t="s">
-        <v>45</v>
-      </c>
-      <c r="X6" s="102" t="s">
+      <c r="V6" s="100" t="s">
+        <v>47</v>
+      </c>
+      <c r="W6" s="99" t="s">
         <v>46</v>
       </c>
-      <c r="Y6" s="102"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75">
+      <c r="X6" s="100" t="s">
+        <v>47</v>
+      </c>
+      <c r="Y6" s="100"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="23.25">
       <c r="A7" s="4"/>
       <c r="B7" s="4"/>
       <c r="C7" s="4"/>
       <c r="D7" s="4"/>
-      <c r="E7" s="101">
+      <c r="E7" s="99">
         <v>71</v>
       </c>
-      <c r="F7" s="102">
+      <c r="F7" s="100">
         <v>3.8</v>
       </c>
-      <c r="G7" s="101">
-        <v>68</v>
-      </c>
-      <c r="H7" s="102">
+      <c r="G7" s="99">
+        <v>68</v>
+      </c>
+      <c r="H7" s="100">
         <v>3.9</v>
       </c>
-      <c r="I7" s="101">
+      <c r="I7" s="99">
         <v>69</v>
       </c>
-      <c r="J7" s="102">
+      <c r="J7" s="100">
         <v>4.2</v>
       </c>
-      <c r="K7" s="101">
+      <c r="K7" s="99">
         <v>69</v>
       </c>
-      <c r="L7" s="102">
+      <c r="L7" s="100">
         <v>4.2</v>
       </c>
-      <c r="M7" s="105"/>
-      <c r="N7" s="106"/>
-      <c r="O7" s="101">
+      <c r="M7" s="103"/>
+      <c r="N7" s="104"/>
+      <c r="O7" s="99">
         <v>71</v>
       </c>
-      <c r="P7" s="102">
+      <c r="P7" s="100">
         <v>3.9</v>
       </c>
-      <c r="Q7" s="101">
+      <c r="Q7" s="99">
         <v>70</v>
       </c>
-      <c r="R7" s="102">
+      <c r="R7" s="100">
         <v>4.7</v>
       </c>
-      <c r="S7" s="101">
+      <c r="S7" s="99">
         <v>70</v>
       </c>
-      <c r="T7" s="102">
+      <c r="T7" s="100">
         <v>4.9</v>
       </c>
-      <c r="U7" s="101">
+      <c r="U7" s="99">
         <v>71</v>
       </c>
-      <c r="V7" s="102">
+      <c r="V7" s="100">
         <v>4.2</v>
       </c>
-      <c r="W7" s="101">
+      <c r="W7" s="99">
         <v>71</v>
       </c>
-      <c r="X7" s="102">
+      <c r="X7" s="100">
         <v>4.3</v>
       </c>
-      <c r="Y7" s="102"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18.75">
+      <c r="Y7" s="100"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="23.25">
       <c r="A8" s="4"/>
       <c r="B8" s="4"/>
       <c r="C8" s="4"/>
       <c r="D8" s="4"/>
-      <c r="E8" s="101">
+      <c r="E8" s="99">
         <v>70</v>
       </c>
-      <c r="F8" s="102">
+      <c r="F8" s="100">
         <v>3.7</v>
       </c>
-      <c r="G8" s="101">
-        <v>68</v>
-      </c>
-      <c r="H8" s="102">
+      <c r="G8" s="99">
+        <v>68</v>
+      </c>
+      <c r="H8" s="100">
         <v>3.9</v>
       </c>
-      <c r="I8" s="101">
-        <v>68</v>
-      </c>
-      <c r="J8" s="102">
+      <c r="I8" s="99">
+        <v>68</v>
+      </c>
+      <c r="J8" s="100">
         <v>4.4</v>
       </c>
-      <c r="K8" s="101">
+      <c r="K8" s="99">
         <v>69</v>
       </c>
-      <c r="L8" s="102">
+      <c r="L8" s="100">
         <v>4.1</v>
       </c>
-      <c r="M8" s="105"/>
-      <c r="N8" s="106"/>
-      <c r="O8" s="101">
+      <c r="M8" s="103"/>
+      <c r="N8" s="104"/>
+      <c r="O8" s="99">
         <v>70</v>
       </c>
-      <c r="P8" s="102">
+      <c r="P8" s="100">
         <v>4.2</v>
       </c>
-      <c r="Q8" s="101">
+      <c r="Q8" s="99">
         <v>70</v>
       </c>
-      <c r="R8" s="102">
+      <c r="R8" s="100">
         <v>4.8</v>
       </c>
-      <c r="S8" s="101">
+      <c r="S8" s="99">
         <v>70</v>
       </c>
-      <c r="T8" s="102">
+      <c r="T8" s="100">
         <v>4.8</v>
       </c>
-      <c r="U8" s="101">
+      <c r="U8" s="99">
         <v>71</v>
       </c>
-      <c r="V8" s="102">
+      <c r="V8" s="100">
         <v>4.1</v>
       </c>
-      <c r="W8" s="101">
+      <c r="W8" s="99">
         <v>70</v>
       </c>
-      <c r="X8" s="102">
+      <c r="X8" s="100">
         <v>4.2</v>
       </c>
-      <c r="Y8" s="102"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18.75">
+      <c r="Y8" s="100"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="23.25">
       <c r="A9" s="4"/>
       <c r="B9" s="4"/>
       <c r="C9" s="4"/>
       <c r="D9" s="4"/>
-      <c r="E9" s="101">
+      <c r="E9" s="99">
         <v>70</v>
       </c>
-      <c r="F9" s="102">
+      <c r="F9" s="100">
         <v>3.8</v>
       </c>
-      <c r="G9" s="101">
+      <c r="G9" s="99">
         <v>69</v>
       </c>
-      <c r="H9" s="102">
+      <c r="H9" s="100">
         <v>3.8</v>
       </c>
-      <c r="I9" s="101">
+      <c r="I9" s="99">
         <v>67</v>
       </c>
-      <c r="J9" s="102">
+      <c r="J9" s="100">
         <v>4.6</v>
       </c>
-      <c r="K9" s="101">
-        <v>68</v>
-      </c>
-      <c r="L9" s="102">
+      <c r="K9" s="99">
+        <v>68</v>
+      </c>
+      <c r="L9" s="100">
         <v>4.1</v>
       </c>
-      <c r="M9" s="105"/>
-      <c r="N9" s="106"/>
-      <c r="O9" s="101">
+      <c r="M9" s="103"/>
+      <c r="N9" s="104"/>
+      <c r="O9" s="99">
         <v>70</v>
       </c>
-      <c r="P9" s="102">
+      <c r="P9" s="100">
         <v>3.9</v>
       </c>
-      <c r="Q9" s="101">
+      <c r="Q9" s="99">
         <v>69</v>
       </c>
-      <c r="R9" s="102">
+      <c r="R9" s="100">
         <v>4.7</v>
       </c>
-      <c r="S9" s="101">
+      <c r="S9" s="99">
         <v>70</v>
       </c>
-      <c r="T9" s="102">
+      <c r="T9" s="100">
         <v>4.9</v>
       </c>
-      <c r="U9" s="101">
+      <c r="U9" s="99">
         <v>70</v>
       </c>
-      <c r="V9" s="102">
+      <c r="V9" s="100">
         <v>4.3</v>
       </c>
-      <c r="W9" s="101">
+      <c r="W9" s="99">
         <v>70</v>
       </c>
-      <c r="X9" s="102">
+      <c r="X9" s="100">
         <v>4.3</v>
       </c>
-      <c r="Y9" s="102"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="18.75">
+      <c r="Y9" s="100"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="23.25">
       <c r="A10" s="4"/>
       <c r="B10" s="4"/>
       <c r="C10" s="4"/>
       <c r="D10" s="4"/>
-      <c r="E10" s="101">
+      <c r="E10" s="99">
         <v>70</v>
       </c>
-      <c r="F10" s="102">
+      <c r="F10" s="100">
         <v>3.8</v>
       </c>
-      <c r="G10" s="101">
-        <v>68</v>
-      </c>
-      <c r="H10" s="102">
+      <c r="G10" s="99">
+        <v>68</v>
+      </c>
+      <c r="H10" s="100">
         <v>3.7</v>
       </c>
-      <c r="I10" s="101">
-        <v>68</v>
-      </c>
-      <c r="J10" s="102">
+      <c r="I10" s="99">
+        <v>68</v>
+      </c>
+      <c r="J10" s="100">
         <v>4.5</v>
       </c>
-      <c r="K10" s="101">
-        <v>68</v>
-      </c>
-      <c r="L10" s="102">
+      <c r="K10" s="99">
+        <v>68</v>
+      </c>
+      <c r="L10" s="100">
         <v>4.2</v>
       </c>
-      <c r="M10" s="105"/>
-      <c r="N10" s="106"/>
-      <c r="O10" s="101">
+      <c r="M10" s="103"/>
+      <c r="N10" s="104"/>
+      <c r="O10" s="99">
         <v>70</v>
       </c>
-      <c r="P10" s="101">
+      <c r="P10" s="99">
         <v>4</v>
       </c>
-      <c r="Q10" s="101">
+      <c r="Q10" s="99">
         <v>69</v>
       </c>
-      <c r="R10" s="101">
+      <c r="R10" s="99">
         <v>5</v>
       </c>
-      <c r="S10" s="101">
+      <c r="S10" s="99">
         <v>70</v>
       </c>
-      <c r="T10" s="102">
+      <c r="T10" s="100">
         <v>4.8</v>
       </c>
-      <c r="U10" s="101">
+      <c r="U10" s="99">
         <v>70</v>
       </c>
-      <c r="V10" s="102">
+      <c r="V10" s="100">
         <v>4.1</v>
       </c>
-      <c r="W10" s="101">
+      <c r="W10" s="99">
         <v>70</v>
       </c>
-      <c r="X10" s="102">
+      <c r="X10" s="100">
         <v>4.2</v>
       </c>
-      <c r="Y10" s="102"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="18.75">
+      <c r="Y10" s="100"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="23.25">
       <c r="A11" s="4"/>
       <c r="B11" s="4"/>
       <c r="C11" s="4"/>
       <c r="D11" s="4"/>
-      <c r="E11" s="101">
+      <c r="E11" s="99">
         <v>69</v>
       </c>
-      <c r="F11" s="102">
+      <c r="F11" s="100">
         <v>3.7</v>
       </c>
-      <c r="G11" s="101">
-        <v>68</v>
-      </c>
-      <c r="H11" s="102">
+      <c r="G11" s="99">
+        <v>68</v>
+      </c>
+      <c r="H11" s="100">
         <v>3.9</v>
       </c>
-      <c r="I11" s="101">
-        <v>68</v>
-      </c>
-      <c r="J11" s="102">
+      <c r="I11" s="99">
+        <v>68</v>
+      </c>
+      <c r="J11" s="100">
         <v>4.3</v>
       </c>
-      <c r="K11" s="101">
-        <v>68</v>
-      </c>
-      <c r="L11" s="102">
+      <c r="K11" s="99">
+        <v>68</v>
+      </c>
+      <c r="L11" s="100">
         <v>4.2</v>
       </c>
-      <c r="M11" s="105"/>
-      <c r="N11" s="106"/>
-      <c r="O11" s="101">
+      <c r="M11" s="103"/>
+      <c r="N11" s="104"/>
+      <c r="O11" s="99">
         <v>69</v>
       </c>
-      <c r="P11" s="101">
+      <c r="P11" s="99">
         <v>4</v>
       </c>
-      <c r="Q11" s="101">
+      <c r="Q11" s="99">
         <v>69</v>
       </c>
-      <c r="R11" s="102">
+      <c r="R11" s="100">
         <v>5.1</v>
       </c>
-      <c r="S11" s="101">
+      <c r="S11" s="99">
         <v>70</v>
       </c>
-      <c r="T11" s="102">
+      <c r="T11" s="100">
         <v>4.6</v>
       </c>
-      <c r="U11" s="101">
+      <c r="U11" s="99">
         <v>71</v>
       </c>
-      <c r="V11" s="102">
+      <c r="V11" s="100">
         <v>4.4</v>
       </c>
-      <c r="W11" s="101">
+      <c r="W11" s="99">
         <v>71</v>
       </c>
-      <c r="X11" s="102">
+      <c r="X11" s="100">
         <v>4.1</v>
       </c>
-      <c r="Y11" s="102"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="18.75">
+      <c r="Y11" s="100"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="24">
       <c r="A12" s="4"/>
       <c r="B12" s="4"/>
       <c r="C12" s="4"/>
       <c r="D12" s="4"/>
-      <c r="E12" s="101">
+      <c r="E12" s="99">
         <f>AVERAGE(E7:E11)</f>
       </c>
-      <c r="F12" s="102">
+      <c r="F12" s="100">
         <f>AVERAGE(F7:F11)</f>
       </c>
-      <c r="G12" s="102">
+      <c r="G12" s="100">
         <f>AVERAGE(G7:G11)</f>
       </c>
-      <c r="H12" s="102">
+      <c r="H12" s="100">
         <f>AVERAGE(H7:H11)</f>
       </c>
-      <c r="I12" s="101">
+      <c r="I12" s="99">
         <f>AVERAGE(I7:I11)</f>
       </c>
-      <c r="J12" s="102">
+      <c r="J12" s="100">
         <f>AVERAGE(J7:J11)</f>
       </c>
-      <c r="K12" s="102">
+      <c r="K12" s="100">
         <f>AVERAGE(K7:K11)</f>
       </c>
-      <c r="L12" s="102">
+      <c r="L12" s="100">
         <f>AVERAGE(L7:L11)</f>
       </c>
-      <c r="M12" s="102">
+      <c r="M12" s="100">
         <f>(F12+H12+J12+L12)/4</f>
       </c>
       <c r="N12" s="4"/>
-      <c r="O12" s="101">
+      <c r="O12" s="99">
         <f>AVERAGE(O7:O11)</f>
       </c>
-      <c r="P12" s="101">
+      <c r="P12" s="99">
         <f>AVERAGE(P7:P11)</f>
       </c>
-      <c r="Q12" s="102">
+      <c r="Q12" s="100">
         <f>AVERAGE(Q7:Q11)</f>
       </c>
-      <c r="R12" s="102">
+      <c r="R12" s="100">
         <f>AVERAGE(R7:R11)</f>
       </c>
-      <c r="S12" s="101">
+      <c r="S12" s="99">
         <f>AVERAGE(S7:S11)</f>
       </c>
-      <c r="T12" s="102">
+      <c r="T12" s="100">
         <f>AVERAGE(T7:T11)</f>
       </c>
-      <c r="U12" s="102">
+      <c r="U12" s="100">
         <f>AVERAGE(U7:U11)</f>
       </c>
-      <c r="V12" s="102">
+      <c r="V12" s="100">
         <f>AVERAGE(V7:V11)</f>
       </c>
-      <c r="W12" s="102">
+      <c r="W12" s="100">
         <f>AVERAGE(W7:W11)</f>
       </c>
-      <c r="X12" s="102">
+      <c r="X12" s="100">
         <f>AVERAGE(X7:X11)</f>
       </c>
-      <c r="Y12" s="102">
+      <c r="Y12" s="100">
         <f>(P12+R12+T12+V12+X12)/5</f>
       </c>
     </row>
@@ -1878,67 +1869,67 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="41" width="24.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="93" width="32.86214285714286" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="93" width="15.719285714285713" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="94" width="15.719285714285713" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="93" width="15.719285714285713" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="94" width="15.719285714285713" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="93" width="15.719285714285713" customWidth="1" bestFit="1"/>
-    <col min="8" max="8" style="94" width="15.719285714285713" customWidth="1" bestFit="1"/>
-    <col min="9" max="9" style="94" width="15.719285714285713" customWidth="1" bestFit="1"/>
-    <col min="10" max="10" style="94" width="15.719285714285713" customWidth="1" bestFit="1"/>
-    <col min="11" max="11" style="94" width="15.719285714285713" customWidth="1" bestFit="1"/>
-    <col min="12" max="12" style="94" width="15.719285714285713" customWidth="1" bestFit="1"/>
-    <col min="13" max="13" style="94" width="15.719285714285713" customWidth="1" bestFit="1"/>
-    <col min="14" max="14" style="94" width="15.719285714285713" customWidth="1" bestFit="1"/>
-    <col min="15" max="15" style="41" width="15.719285714285713" customWidth="1" bestFit="1"/>
-    <col min="16" max="16" style="41" width="64.29071428571429" customWidth="1" bestFit="1"/>
-    <col min="17" max="17" style="41" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="18" max="18" style="41" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="19" max="19" style="41" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="20" max="20" style="41" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="21" max="21" style="41" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="22" max="22" style="41" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="23" max="23" style="41" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="24" max="24" style="41" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="25" max="25" style="41" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="26" max="26" style="41" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="27" max="27" style="41" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="28" max="28" style="41" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="29" max="29" style="41" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="30" max="30" style="41" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="31" max="31" style="41" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="32" max="32" style="41" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="33" max="33" style="41" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="34" max="34" style="41" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="35" max="35" style="41" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="36" max="36" style="41" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="37" max="37" style="41" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="38" max="38" style="41" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="39" max="39" style="41" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="40" max="40" style="41" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="41" max="41" style="41" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="42" max="42" style="41" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="43" max="43" style="41" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="44" max="44" style="41" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="40" width="24.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="91" width="32.86214285714286" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="91" width="15.719285714285713" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="92" width="15.719285714285713" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="91" width="15.719285714285713" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="92" width="15.719285714285713" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="91" width="15.719285714285713" customWidth="1" bestFit="1"/>
+    <col min="8" max="8" style="92" width="15.719285714285713" customWidth="1" bestFit="1"/>
+    <col min="9" max="9" style="92" width="15.719285714285713" customWidth="1" bestFit="1"/>
+    <col min="10" max="10" style="92" width="15.719285714285713" customWidth="1" bestFit="1"/>
+    <col min="11" max="11" style="92" width="15.719285714285713" customWidth="1" bestFit="1"/>
+    <col min="12" max="12" style="92" width="15.719285714285713" customWidth="1" bestFit="1"/>
+    <col min="13" max="13" style="92" width="15.719285714285713" customWidth="1" bestFit="1"/>
+    <col min="14" max="14" style="92" width="15.719285714285713" customWidth="1" bestFit="1"/>
+    <col min="15" max="15" style="40" width="15.719285714285713" customWidth="1" bestFit="1"/>
+    <col min="16" max="16" style="40" width="64.29071428571429" customWidth="1" bestFit="1"/>
+    <col min="17" max="17" style="40" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="18" max="18" style="40" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="19" max="19" style="40" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="20" max="20" style="40" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="21" max="21" style="40" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="22" max="22" style="40" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="23" max="23" style="40" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="24" max="24" style="40" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="25" max="25" style="40" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="26" max="26" style="40" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="27" max="27" style="40" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="28" max="28" style="40" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="29" max="29" style="40" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="30" max="30" style="40" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="31" max="31" style="40" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="32" max="32" style="40" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="33" max="33" style="40" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="34" max="34" style="40" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="35" max="35" style="40" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="36" max="36" style="40" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="37" max="37" style="40" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="38" max="38" style="40" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="39" max="39" style="40" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="40" max="40" style="40" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="41" max="41" style="40" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="42" max="42" style="40" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="43" max="43" style="40" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="44" max="44" style="40" width="13.576428571428572" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
       <c r="A1" s="4"/>
-      <c r="B1" s="69"/>
-      <c r="C1" s="69"/>
-      <c r="D1" s="70"/>
-      <c r="E1" s="69"/>
-      <c r="F1" s="70"/>
-      <c r="G1" s="69"/>
-      <c r="H1" s="70"/>
-      <c r="I1" s="70"/>
-      <c r="J1" s="70"/>
-      <c r="K1" s="70"/>
-      <c r="L1" s="70"/>
-      <c r="M1" s="70"/>
-      <c r="N1" s="70"/>
+      <c r="B1" s="70"/>
+      <c r="C1" s="70"/>
+      <c r="D1" s="71"/>
+      <c r="E1" s="70"/>
+      <c r="F1" s="71"/>
+      <c r="G1" s="70"/>
+      <c r="H1" s="71"/>
+      <c r="I1" s="71"/>
+      <c r="J1" s="71"/>
+      <c r="K1" s="71"/>
+      <c r="L1" s="71"/>
+      <c r="M1" s="71"/>
+      <c r="N1" s="71"/>
       <c r="O1" s="4"/>
       <c r="P1" s="4"/>
       <c r="Q1" s="4"/>
@@ -1971,22 +1962,22 @@
       <c r="AR1" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
-      <c r="A2" s="71" t="s">
-        <v>31</v>
-      </c>
-      <c r="B2" s="72"/>
-      <c r="C2" s="72"/>
-      <c r="D2" s="73"/>
-      <c r="E2" s="72"/>
-      <c r="F2" s="73"/>
-      <c r="G2" s="72"/>
-      <c r="H2" s="73"/>
-      <c r="I2" s="73"/>
-      <c r="J2" s="73"/>
-      <c r="K2" s="73"/>
-      <c r="L2" s="73"/>
-      <c r="M2" s="73"/>
-      <c r="N2" s="73"/>
+      <c r="A2" s="72" t="s">
+        <v>32</v>
+      </c>
+      <c r="B2" s="73"/>
+      <c r="C2" s="73"/>
+      <c r="D2" s="74"/>
+      <c r="E2" s="73"/>
+      <c r="F2" s="74"/>
+      <c r="G2" s="73"/>
+      <c r="H2" s="74"/>
+      <c r="I2" s="74"/>
+      <c r="J2" s="74"/>
+      <c r="K2" s="74"/>
+      <c r="L2" s="74"/>
+      <c r="M2" s="74"/>
+      <c r="N2" s="74"/>
       <c r="O2" s="4"/>
       <c r="P2" s="4"/>
       <c r="Q2" s="4"/>
@@ -2072,27 +2063,27 @@
       <c r="C4" s="47" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="74"/>
+      <c r="D4" s="75"/>
       <c r="E4" s="47" t="s">
         <v>1</v>
       </c>
-      <c r="F4" s="74"/>
+      <c r="F4" s="75"/>
       <c r="G4" s="47" t="s">
         <v>2</v>
       </c>
-      <c r="H4" s="74"/>
-      <c r="I4" s="75" t="s">
+      <c r="H4" s="75"/>
+      <c r="I4" s="76" t="s">
         <v>3</v>
       </c>
-      <c r="J4" s="74"/>
-      <c r="K4" s="75" t="s">
+      <c r="J4" s="75"/>
+      <c r="K4" s="76" t="s">
         <v>4</v>
       </c>
-      <c r="L4" s="74"/>
-      <c r="M4" s="76" t="s">
+      <c r="L4" s="75"/>
+      <c r="M4" s="77" t="s">
         <v>5</v>
       </c>
-      <c r="N4" s="76"/>
+      <c r="N4" s="77"/>
       <c r="O4" s="9"/>
       <c r="P4" s="9" t="s">
         <v>12</v>
@@ -2135,7 +2126,7 @@
         <v>8</v>
       </c>
       <c r="D5" s="45" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="E5" s="46" t="s">
         <v>10</v>
@@ -2273,7 +2264,7 @@
       <c r="AR6" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75">
-      <c r="A7" s="77"/>
+      <c r="A7" s="78"/>
       <c r="B7" s="49">
         <v>2</v>
       </c>
@@ -2345,7 +2336,7 @@
       <c r="AR7" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18.75">
-      <c r="A8" s="77"/>
+      <c r="A8" s="78"/>
       <c r="B8" s="49">
         <v>3</v>
       </c>
@@ -2417,7 +2408,7 @@
       <c r="AR8" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18.75">
-      <c r="A9" s="77"/>
+      <c r="A9" s="78"/>
       <c r="B9" s="49">
         <v>4</v>
       </c>
@@ -2489,7 +2480,7 @@
       <c r="AR9" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="18.75">
-      <c r="A10" s="77"/>
+      <c r="A10" s="78"/>
       <c r="B10" s="49">
         <v>5</v>
       </c>
@@ -2634,19 +2625,19 @@
     </row>
     <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="18.75">
       <c r="A12" s="9"/>
-      <c r="B12" s="78"/>
-      <c r="C12" s="79"/>
-      <c r="D12" s="80"/>
-      <c r="E12" s="79"/>
-      <c r="F12" s="80"/>
-      <c r="G12" s="79"/>
-      <c r="H12" s="80"/>
-      <c r="I12" s="80"/>
-      <c r="J12" s="80"/>
-      <c r="K12" s="80"/>
-      <c r="L12" s="80"/>
-      <c r="M12" s="80"/>
-      <c r="N12" s="80"/>
+      <c r="B12" s="79"/>
+      <c r="C12" s="80"/>
+      <c r="D12" s="81"/>
+      <c r="E12" s="80"/>
+      <c r="F12" s="81"/>
+      <c r="G12" s="80"/>
+      <c r="H12" s="81"/>
+      <c r="I12" s="81"/>
+      <c r="J12" s="81"/>
+      <c r="K12" s="81"/>
+      <c r="L12" s="81"/>
+      <c r="M12" s="81"/>
+      <c r="N12" s="81"/>
       <c r="O12" s="9"/>
       <c r="P12" s="9"/>
       <c r="Q12" s="9"/>
@@ -2726,7 +2717,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="18.75">
       <c r="A14" s="9"/>
-      <c r="B14" s="81"/>
+      <c r="B14" s="82"/>
       <c r="C14" s="2"/>
       <c r="D14" s="3"/>
       <c r="E14" s="2"/>
@@ -2740,8 +2731,8 @@
       <c r="M14" s="3"/>
       <c r="N14" s="3"/>
       <c r="O14" s="9"/>
-      <c r="P14" s="82"/>
-      <c r="Q14" s="82"/>
+      <c r="P14" s="9"/>
+      <c r="Q14" s="9"/>
       <c r="R14" s="9"/>
       <c r="S14" s="83"/>
       <c r="T14" s="83"/>
@@ -2772,7 +2763,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="18.75">
       <c r="A15" s="9"/>
-      <c r="B15" s="81"/>
+      <c r="B15" s="82"/>
       <c r="C15" s="5" t="s">
         <v>17</v>
       </c>
@@ -2792,8 +2783,8 @@
       <c r="M15" s="7"/>
       <c r="N15" s="6"/>
       <c r="O15" s="9"/>
-      <c r="P15" s="82"/>
-      <c r="Q15" s="82"/>
+      <c r="P15" s="9"/>
+      <c r="Q15" s="9"/>
       <c r="R15" s="9"/>
       <c r="S15" s="83"/>
       <c r="T15" s="83"/>
@@ -2954,7 +2945,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="21">
       <c r="A18" s="48" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B18" s="49">
         <v>1</v>
@@ -3500,14 +3491,14 @@
       <c r="M26" s="45"/>
       <c r="N26" s="45"/>
       <c r="O26" s="9"/>
-      <c r="P26" s="82"/>
-      <c r="Q26" s="82"/>
+      <c r="P26" s="9"/>
+      <c r="Q26" s="9"/>
       <c r="R26" s="9"/>
       <c r="S26" s="9"/>
-      <c r="T26" s="82"/>
-      <c r="U26" s="82"/>
-      <c r="V26" s="82"/>
-      <c r="W26" s="82"/>
+      <c r="T26" s="9"/>
+      <c r="U26" s="9"/>
+      <c r="V26" s="9"/>
+      <c r="W26" s="9"/>
       <c r="X26" s="9"/>
       <c r="Y26" s="9"/>
       <c r="Z26" s="9"/>
@@ -3662,7 +3653,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="29" customHeight="1" ht="20.45">
       <c r="A29" s="48" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B29" s="49">
         <v>1</v>
@@ -4194,28 +4185,28 @@
       </c>
       <c r="D37" s="88"/>
       <c r="E37" s="89"/>
-      <c r="F37" s="74"/>
+      <c r="F37" s="75"/>
       <c r="G37" s="47" t="s">
         <v>18</v>
       </c>
       <c r="H37" s="88"/>
       <c r="I37" s="88"/>
-      <c r="J37" s="74"/>
-      <c r="K37" s="75" t="s">
+      <c r="J37" s="75"/>
+      <c r="K37" s="76" t="s">
         <v>19</v>
       </c>
       <c r="L37" s="88"/>
       <c r="M37" s="88"/>
       <c r="N37" s="88"/>
       <c r="O37" s="9"/>
-      <c r="P37" s="82"/>
-      <c r="Q37" s="82"/>
+      <c r="P37" s="9"/>
+      <c r="Q37" s="9"/>
       <c r="R37" s="9"/>
       <c r="S37" s="9"/>
-      <c r="T37" s="82"/>
-      <c r="U37" s="82"/>
-      <c r="V37" s="82"/>
-      <c r="W37" s="82"/>
+      <c r="T37" s="9"/>
+      <c r="U37" s="9"/>
+      <c r="V37" s="9"/>
+      <c r="W37" s="9"/>
       <c r="X37" s="9"/>
       <c r="Y37" s="9"/>
       <c r="Z37" s="9"/>
@@ -4370,7 +4361,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="40" customHeight="1" ht="27">
       <c r="A40" s="48" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B40" s="49">
         <v>1</v>
@@ -4920,10 +4911,10 @@
       <c r="Q48" s="9"/>
       <c r="R48" s="9"/>
       <c r="S48" s="9"/>
-      <c r="T48" s="82"/>
-      <c r="U48" s="82"/>
-      <c r="V48" s="82"/>
-      <c r="W48" s="82"/>
+      <c r="T48" s="9"/>
+      <c r="U48" s="9"/>
+      <c r="V48" s="9"/>
+      <c r="W48" s="9"/>
       <c r="X48" s="9"/>
       <c r="Y48" s="9"/>
       <c r="Z48" s="9"/>
@@ -5078,7 +5069,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="51" customHeight="1" ht="23.45">
       <c r="A51" s="48" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B51" s="49">
         <v>1</v>
@@ -5786,7 +5777,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="62" customHeight="1" ht="18.75">
       <c r="A62" s="48" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B62" s="49">
         <v>1</v>
@@ -6266,14 +6257,14 @@
     </row>
     <row x14ac:dyDescent="0.25" r="69" customHeight="1" ht="18.75">
       <c r="A69" s="9"/>
-      <c r="B69" s="91"/>
-      <c r="C69" s="91"/>
+      <c r="B69" s="44"/>
+      <c r="C69" s="44"/>
       <c r="D69" s="58"/>
       <c r="E69" s="44"/>
-      <c r="F69" s="92"/>
-      <c r="G69" s="91"/>
-      <c r="H69" s="92"/>
-      <c r="I69" s="92"/>
+      <c r="F69" s="58"/>
+      <c r="G69" s="44"/>
+      <c r="H69" s="58"/>
+      <c r="I69" s="58"/>
       <c r="J69" s="58"/>
       <c r="K69" s="58"/>
       <c r="L69" s="58"/>
@@ -6312,14 +6303,14 @@
     </row>
     <row x14ac:dyDescent="0.25" r="70" customHeight="1" ht="18.75">
       <c r="A70" s="9"/>
-      <c r="B70" s="91"/>
-      <c r="C70" s="91"/>
+      <c r="B70" s="44"/>
+      <c r="C70" s="44"/>
       <c r="D70" s="58"/>
       <c r="E70" s="44"/>
-      <c r="F70" s="92"/>
-      <c r="G70" s="91"/>
-      <c r="H70" s="92"/>
-      <c r="I70" s="92"/>
+      <c r="F70" s="58"/>
+      <c r="G70" s="44"/>
+      <c r="H70" s="58"/>
+      <c r="I70" s="58"/>
       <c r="J70" s="58"/>
       <c r="K70" s="58"/>
       <c r="L70" s="58"/>
@@ -6358,14 +6349,14 @@
     </row>
     <row x14ac:dyDescent="0.25" r="71" customHeight="1" ht="18.75">
       <c r="A71" s="9"/>
-      <c r="B71" s="91"/>
-      <c r="C71" s="91"/>
+      <c r="B71" s="44"/>
+      <c r="C71" s="44"/>
       <c r="D71" s="58"/>
       <c r="E71" s="44"/>
-      <c r="F71" s="92"/>
-      <c r="G71" s="91"/>
-      <c r="H71" s="92"/>
-      <c r="I71" s="92"/>
+      <c r="F71" s="58"/>
+      <c r="G71" s="44"/>
+      <c r="H71" s="58"/>
+      <c r="I71" s="58"/>
       <c r="J71" s="58"/>
       <c r="K71" s="58"/>
       <c r="L71" s="58"/>
@@ -6404,19 +6395,19 @@
     </row>
     <row x14ac:dyDescent="0.25" r="72" customHeight="1" ht="18.75">
       <c r="A72" s="4"/>
-      <c r="B72" s="69"/>
-      <c r="C72" s="69"/>
-      <c r="D72" s="70"/>
-      <c r="E72" s="69"/>
-      <c r="F72" s="70"/>
-      <c r="G72" s="69"/>
-      <c r="H72" s="70"/>
-      <c r="I72" s="70"/>
-      <c r="J72" s="70"/>
-      <c r="K72" s="70"/>
-      <c r="L72" s="70"/>
-      <c r="M72" s="70"/>
-      <c r="N72" s="70"/>
+      <c r="B72" s="70"/>
+      <c r="C72" s="70"/>
+      <c r="D72" s="71"/>
+      <c r="E72" s="70"/>
+      <c r="F72" s="71"/>
+      <c r="G72" s="70"/>
+      <c r="H72" s="71"/>
+      <c r="I72" s="71"/>
+      <c r="J72" s="71"/>
+      <c r="K72" s="71"/>
+      <c r="L72" s="71"/>
+      <c r="M72" s="71"/>
+      <c r="N72" s="71"/>
       <c r="O72" s="4"/>
       <c r="P72" s="4"/>
       <c r="Q72" s="4"/>
@@ -6450,19 +6441,19 @@
     </row>
     <row x14ac:dyDescent="0.25" r="73" customHeight="1" ht="18.75">
       <c r="A73" s="4"/>
-      <c r="B73" s="69"/>
-      <c r="C73" s="69"/>
-      <c r="D73" s="70"/>
-      <c r="E73" s="69"/>
-      <c r="F73" s="70"/>
-      <c r="G73" s="69"/>
-      <c r="H73" s="70"/>
-      <c r="I73" s="70"/>
-      <c r="J73" s="70"/>
-      <c r="K73" s="70"/>
-      <c r="L73" s="70"/>
-      <c r="M73" s="70"/>
-      <c r="N73" s="70"/>
+      <c r="B73" s="70"/>
+      <c r="C73" s="70"/>
+      <c r="D73" s="71"/>
+      <c r="E73" s="70"/>
+      <c r="F73" s="71"/>
+      <c r="G73" s="70"/>
+      <c r="H73" s="71"/>
+      <c r="I73" s="71"/>
+      <c r="J73" s="71"/>
+      <c r="K73" s="71"/>
+      <c r="L73" s="71"/>
+      <c r="M73" s="71"/>
+      <c r="N73" s="71"/>
       <c r="O73" s="4"/>
       <c r="P73" s="4"/>
       <c r="Q73" s="4"/>
@@ -6496,19 +6487,19 @@
     </row>
     <row x14ac:dyDescent="0.25" r="74" customHeight="1" ht="18.75">
       <c r="A74" s="4"/>
-      <c r="B74" s="69"/>
-      <c r="C74" s="69"/>
-      <c r="D74" s="70"/>
-      <c r="E74" s="69"/>
-      <c r="F74" s="70"/>
-      <c r="G74" s="69"/>
-      <c r="H74" s="70"/>
-      <c r="I74" s="70"/>
-      <c r="J74" s="70"/>
-      <c r="K74" s="70"/>
-      <c r="L74" s="70"/>
-      <c r="M74" s="70"/>
-      <c r="N74" s="70"/>
+      <c r="B74" s="70"/>
+      <c r="C74" s="70"/>
+      <c r="D74" s="71"/>
+      <c r="E74" s="70"/>
+      <c r="F74" s="71"/>
+      <c r="G74" s="70"/>
+      <c r="H74" s="71"/>
+      <c r="I74" s="71"/>
+      <c r="J74" s="71"/>
+      <c r="K74" s="71"/>
+      <c r="L74" s="71"/>
+      <c r="M74" s="71"/>
+      <c r="N74" s="71"/>
       <c r="O74" s="4"/>
       <c r="P74" s="4"/>
       <c r="Q74" s="4"/>
@@ -6542,19 +6533,19 @@
     </row>
     <row x14ac:dyDescent="0.25" r="75" customHeight="1" ht="18.75">
       <c r="A75" s="4"/>
-      <c r="B75" s="69"/>
-      <c r="C75" s="69"/>
-      <c r="D75" s="70"/>
-      <c r="E75" s="69"/>
-      <c r="F75" s="70"/>
-      <c r="G75" s="69"/>
-      <c r="H75" s="70"/>
-      <c r="I75" s="70"/>
-      <c r="J75" s="70"/>
-      <c r="K75" s="70"/>
-      <c r="L75" s="70"/>
-      <c r="M75" s="70"/>
-      <c r="N75" s="70"/>
+      <c r="B75" s="70"/>
+      <c r="C75" s="70"/>
+      <c r="D75" s="71"/>
+      <c r="E75" s="70"/>
+      <c r="F75" s="71"/>
+      <c r="G75" s="70"/>
+      <c r="H75" s="71"/>
+      <c r="I75" s="71"/>
+      <c r="J75" s="71"/>
+      <c r="K75" s="71"/>
+      <c r="L75" s="71"/>
+      <c r="M75" s="71"/>
+      <c r="N75" s="71"/>
       <c r="O75" s="4"/>
       <c r="P75" s="4"/>
       <c r="Q75" s="4"/>
@@ -6588,19 +6579,19 @@
     </row>
     <row x14ac:dyDescent="0.25" r="76" customHeight="1" ht="18.75">
       <c r="A76" s="4"/>
-      <c r="B76" s="69"/>
-      <c r="C76" s="69"/>
-      <c r="D76" s="70"/>
-      <c r="E76" s="69"/>
-      <c r="F76" s="70"/>
-      <c r="G76" s="69"/>
-      <c r="H76" s="70"/>
-      <c r="I76" s="70"/>
-      <c r="J76" s="70"/>
-      <c r="K76" s="70"/>
-      <c r="L76" s="70"/>
-      <c r="M76" s="70"/>
-      <c r="N76" s="70"/>
+      <c r="B76" s="70"/>
+      <c r="C76" s="70"/>
+      <c r="D76" s="71"/>
+      <c r="E76" s="70"/>
+      <c r="F76" s="71"/>
+      <c r="G76" s="70"/>
+      <c r="H76" s="71"/>
+      <c r="I76" s="71"/>
+      <c r="J76" s="71"/>
+      <c r="K76" s="71"/>
+      <c r="L76" s="71"/>
+      <c r="M76" s="71"/>
+      <c r="N76" s="71"/>
       <c r="O76" s="4"/>
       <c r="P76" s="4"/>
       <c r="Q76" s="4"/>
@@ -6634,19 +6625,19 @@
     </row>
     <row x14ac:dyDescent="0.25" r="77" customHeight="1" ht="18.75">
       <c r="A77" s="4"/>
-      <c r="B77" s="69"/>
-      <c r="C77" s="69"/>
-      <c r="D77" s="70"/>
-      <c r="E77" s="69"/>
-      <c r="F77" s="70"/>
-      <c r="G77" s="69"/>
-      <c r="H77" s="70"/>
-      <c r="I77" s="70"/>
-      <c r="J77" s="70"/>
-      <c r="K77" s="70"/>
-      <c r="L77" s="70"/>
-      <c r="M77" s="70"/>
-      <c r="N77" s="70"/>
+      <c r="B77" s="70"/>
+      <c r="C77" s="70"/>
+      <c r="D77" s="71"/>
+      <c r="E77" s="70"/>
+      <c r="F77" s="71"/>
+      <c r="G77" s="70"/>
+      <c r="H77" s="71"/>
+      <c r="I77" s="71"/>
+      <c r="J77" s="71"/>
+      <c r="K77" s="71"/>
+      <c r="L77" s="71"/>
+      <c r="M77" s="71"/>
+      <c r="N77" s="71"/>
       <c r="O77" s="4"/>
       <c r="P77" s="4"/>
       <c r="Q77" s="4"/>
@@ -6680,19 +6671,19 @@
     </row>
     <row x14ac:dyDescent="0.25" r="78" customHeight="1" ht="18.75">
       <c r="A78" s="4"/>
-      <c r="B78" s="69"/>
-      <c r="C78" s="69"/>
-      <c r="D78" s="70"/>
-      <c r="E78" s="69"/>
-      <c r="F78" s="70"/>
-      <c r="G78" s="69"/>
-      <c r="H78" s="70"/>
-      <c r="I78" s="70"/>
-      <c r="J78" s="70"/>
-      <c r="K78" s="70"/>
-      <c r="L78" s="70"/>
-      <c r="M78" s="70"/>
-      <c r="N78" s="70"/>
+      <c r="B78" s="70"/>
+      <c r="C78" s="70"/>
+      <c r="D78" s="71"/>
+      <c r="E78" s="70"/>
+      <c r="F78" s="71"/>
+      <c r="G78" s="70"/>
+      <c r="H78" s="71"/>
+      <c r="I78" s="71"/>
+      <c r="J78" s="71"/>
+      <c r="K78" s="71"/>
+      <c r="L78" s="71"/>
+      <c r="M78" s="71"/>
+      <c r="N78" s="71"/>
       <c r="O78" s="4"/>
       <c r="P78" s="4"/>
       <c r="Q78" s="4"/>
@@ -6726,19 +6717,19 @@
     </row>
     <row x14ac:dyDescent="0.25" r="79" customHeight="1" ht="18.75">
       <c r="A79" s="4"/>
-      <c r="B79" s="69"/>
-      <c r="C79" s="69"/>
-      <c r="D79" s="70"/>
-      <c r="E79" s="69"/>
-      <c r="F79" s="70"/>
-      <c r="G79" s="69"/>
-      <c r="H79" s="70"/>
-      <c r="I79" s="70"/>
-      <c r="J79" s="70"/>
-      <c r="K79" s="70"/>
-      <c r="L79" s="70"/>
-      <c r="M79" s="70"/>
-      <c r="N79" s="70"/>
+      <c r="B79" s="70"/>
+      <c r="C79" s="70"/>
+      <c r="D79" s="71"/>
+      <c r="E79" s="70"/>
+      <c r="F79" s="71"/>
+      <c r="G79" s="70"/>
+      <c r="H79" s="71"/>
+      <c r="I79" s="71"/>
+      <c r="J79" s="71"/>
+      <c r="K79" s="71"/>
+      <c r="L79" s="71"/>
+      <c r="M79" s="71"/>
+      <c r="N79" s="71"/>
       <c r="O79" s="4"/>
       <c r="P79" s="4"/>
       <c r="Q79" s="4"/>
@@ -6772,19 +6763,19 @@
     </row>
     <row x14ac:dyDescent="0.25" r="80" customHeight="1" ht="18.75">
       <c r="A80" s="4"/>
-      <c r="B80" s="69"/>
-      <c r="C80" s="69"/>
-      <c r="D80" s="70"/>
-      <c r="E80" s="69"/>
-      <c r="F80" s="70"/>
-      <c r="G80" s="69"/>
-      <c r="H80" s="70"/>
-      <c r="I80" s="70"/>
-      <c r="J80" s="70"/>
-      <c r="K80" s="70"/>
-      <c r="L80" s="70"/>
-      <c r="M80" s="70"/>
-      <c r="N80" s="70"/>
+      <c r="B80" s="70"/>
+      <c r="C80" s="70"/>
+      <c r="D80" s="71"/>
+      <c r="E80" s="70"/>
+      <c r="F80" s="71"/>
+      <c r="G80" s="70"/>
+      <c r="H80" s="71"/>
+      <c r="I80" s="71"/>
+      <c r="J80" s="71"/>
+      <c r="K80" s="71"/>
+      <c r="L80" s="71"/>
+      <c r="M80" s="71"/>
+      <c r="N80" s="71"/>
       <c r="O80" s="4"/>
       <c r="P80" s="4"/>
       <c r="Q80" s="4"/>
@@ -6818,19 +6809,19 @@
     </row>
     <row x14ac:dyDescent="0.25" r="81" customHeight="1" ht="18.75">
       <c r="A81" s="4"/>
-      <c r="B81" s="69"/>
-      <c r="C81" s="69"/>
-      <c r="D81" s="70"/>
-      <c r="E81" s="69"/>
-      <c r="F81" s="70"/>
-      <c r="G81" s="69"/>
-      <c r="H81" s="70"/>
-      <c r="I81" s="70"/>
-      <c r="J81" s="70"/>
-      <c r="K81" s="70"/>
-      <c r="L81" s="70"/>
-      <c r="M81" s="70"/>
-      <c r="N81" s="70"/>
+      <c r="B81" s="70"/>
+      <c r="C81" s="70"/>
+      <c r="D81" s="71"/>
+      <c r="E81" s="70"/>
+      <c r="F81" s="71"/>
+      <c r="G81" s="70"/>
+      <c r="H81" s="71"/>
+      <c r="I81" s="71"/>
+      <c r="J81" s="71"/>
+      <c r="K81" s="71"/>
+      <c r="L81" s="71"/>
+      <c r="M81" s="71"/>
+      <c r="N81" s="71"/>
       <c r="O81" s="4"/>
       <c r="P81" s="4"/>
       <c r="Q81" s="4"/>
@@ -6864,19 +6855,19 @@
     </row>
     <row x14ac:dyDescent="0.25" r="82" customHeight="1" ht="18.75">
       <c r="A82" s="4"/>
-      <c r="B82" s="69"/>
-      <c r="C82" s="69"/>
-      <c r="D82" s="70"/>
-      <c r="E82" s="69"/>
-      <c r="F82" s="70"/>
-      <c r="G82" s="69"/>
-      <c r="H82" s="70"/>
-      <c r="I82" s="70"/>
-      <c r="J82" s="70"/>
-      <c r="K82" s="70"/>
-      <c r="L82" s="70"/>
-      <c r="M82" s="70"/>
-      <c r="N82" s="70"/>
+      <c r="B82" s="70"/>
+      <c r="C82" s="70"/>
+      <c r="D82" s="71"/>
+      <c r="E82" s="70"/>
+      <c r="F82" s="71"/>
+      <c r="G82" s="70"/>
+      <c r="H82" s="71"/>
+      <c r="I82" s="71"/>
+      <c r="J82" s="71"/>
+      <c r="K82" s="71"/>
+      <c r="L82" s="71"/>
+      <c r="M82" s="71"/>
+      <c r="N82" s="71"/>
       <c r="O82" s="4"/>
       <c r="P82" s="4"/>
       <c r="Q82" s="4"/>
@@ -6910,19 +6901,19 @@
     </row>
     <row x14ac:dyDescent="0.25" r="83" customHeight="1" ht="18.75">
       <c r="A83" s="4"/>
-      <c r="B83" s="69"/>
-      <c r="C83" s="69"/>
-      <c r="D83" s="70"/>
-      <c r="E83" s="69"/>
-      <c r="F83" s="70"/>
-      <c r="G83" s="69"/>
-      <c r="H83" s="70"/>
-      <c r="I83" s="70"/>
-      <c r="J83" s="70"/>
-      <c r="K83" s="70"/>
-      <c r="L83" s="70"/>
-      <c r="M83" s="70"/>
-      <c r="N83" s="70"/>
+      <c r="B83" s="70"/>
+      <c r="C83" s="70"/>
+      <c r="D83" s="71"/>
+      <c r="E83" s="70"/>
+      <c r="F83" s="71"/>
+      <c r="G83" s="70"/>
+      <c r="H83" s="71"/>
+      <c r="I83" s="71"/>
+      <c r="J83" s="71"/>
+      <c r="K83" s="71"/>
+      <c r="L83" s="71"/>
+      <c r="M83" s="71"/>
+      <c r="N83" s="71"/>
       <c r="O83" s="4"/>
       <c r="P83" s="4"/>
       <c r="Q83" s="4"/>
@@ -6956,19 +6947,19 @@
     </row>
     <row x14ac:dyDescent="0.25" r="84" customHeight="1" ht="18.75">
       <c r="A84" s="4"/>
-      <c r="B84" s="69"/>
-      <c r="C84" s="69"/>
-      <c r="D84" s="70"/>
-      <c r="E84" s="69"/>
-      <c r="F84" s="70"/>
-      <c r="G84" s="69"/>
-      <c r="H84" s="70"/>
-      <c r="I84" s="70"/>
-      <c r="J84" s="70"/>
-      <c r="K84" s="70"/>
-      <c r="L84" s="70"/>
-      <c r="M84" s="70"/>
-      <c r="N84" s="70"/>
+      <c r="B84" s="70"/>
+      <c r="C84" s="70"/>
+      <c r="D84" s="71"/>
+      <c r="E84" s="70"/>
+      <c r="F84" s="71"/>
+      <c r="G84" s="70"/>
+      <c r="H84" s="71"/>
+      <c r="I84" s="71"/>
+      <c r="J84" s="71"/>
+      <c r="K84" s="71"/>
+      <c r="L84" s="71"/>
+      <c r="M84" s="71"/>
+      <c r="N84" s="71"/>
       <c r="O84" s="4"/>
       <c r="P84" s="4"/>
       <c r="Q84" s="4"/>
@@ -7002,19 +6993,19 @@
     </row>
     <row x14ac:dyDescent="0.25" r="85" customHeight="1" ht="18.75">
       <c r="A85" s="4"/>
-      <c r="B85" s="69"/>
-      <c r="C85" s="69"/>
-      <c r="D85" s="70"/>
-      <c r="E85" s="69"/>
-      <c r="F85" s="70"/>
-      <c r="G85" s="69"/>
-      <c r="H85" s="70"/>
-      <c r="I85" s="70"/>
-      <c r="J85" s="70"/>
-      <c r="K85" s="70"/>
-      <c r="L85" s="70"/>
-      <c r="M85" s="70"/>
-      <c r="N85" s="70"/>
+      <c r="B85" s="70"/>
+      <c r="C85" s="70"/>
+      <c r="D85" s="71"/>
+      <c r="E85" s="70"/>
+      <c r="F85" s="71"/>
+      <c r="G85" s="70"/>
+      <c r="H85" s="71"/>
+      <c r="I85" s="71"/>
+      <c r="J85" s="71"/>
+      <c r="K85" s="71"/>
+      <c r="L85" s="71"/>
+      <c r="M85" s="71"/>
+      <c r="N85" s="71"/>
       <c r="O85" s="4"/>
       <c r="P85" s="4"/>
       <c r="Q85" s="4"/>
@@ -7048,19 +7039,19 @@
     </row>
     <row x14ac:dyDescent="0.25" r="86" customHeight="1" ht="18.75">
       <c r="A86" s="4"/>
-      <c r="B86" s="69"/>
-      <c r="C86" s="69"/>
-      <c r="D86" s="70"/>
-      <c r="E86" s="69"/>
-      <c r="F86" s="70"/>
-      <c r="G86" s="69"/>
-      <c r="H86" s="70"/>
-      <c r="I86" s="70"/>
-      <c r="J86" s="70"/>
-      <c r="K86" s="70"/>
-      <c r="L86" s="70"/>
-      <c r="M86" s="70"/>
-      <c r="N86" s="70"/>
+      <c r="B86" s="70"/>
+      <c r="C86" s="70"/>
+      <c r="D86" s="71"/>
+      <c r="E86" s="70"/>
+      <c r="F86" s="71"/>
+      <c r="G86" s="70"/>
+      <c r="H86" s="71"/>
+      <c r="I86" s="71"/>
+      <c r="J86" s="71"/>
+      <c r="K86" s="71"/>
+      <c r="L86" s="71"/>
+      <c r="M86" s="71"/>
+      <c r="N86" s="71"/>
       <c r="O86" s="4"/>
       <c r="P86" s="4"/>
       <c r="Q86" s="4"/>
@@ -7094,19 +7085,19 @@
     </row>
     <row x14ac:dyDescent="0.25" r="87" customHeight="1" ht="18.75">
       <c r="A87" s="4"/>
-      <c r="B87" s="69"/>
-      <c r="C87" s="69"/>
-      <c r="D87" s="70"/>
-      <c r="E87" s="69"/>
-      <c r="F87" s="70"/>
-      <c r="G87" s="69"/>
-      <c r="H87" s="70"/>
-      <c r="I87" s="70"/>
-      <c r="J87" s="70"/>
-      <c r="K87" s="70"/>
-      <c r="L87" s="70"/>
-      <c r="M87" s="70"/>
-      <c r="N87" s="70"/>
+      <c r="B87" s="70"/>
+      <c r="C87" s="70"/>
+      <c r="D87" s="71"/>
+      <c r="E87" s="70"/>
+      <c r="F87" s="71"/>
+      <c r="G87" s="70"/>
+      <c r="H87" s="71"/>
+      <c r="I87" s="71"/>
+      <c r="J87" s="71"/>
+      <c r="K87" s="71"/>
+      <c r="L87" s="71"/>
+      <c r="M87" s="71"/>
+      <c r="N87" s="71"/>
       <c r="O87" s="4"/>
       <c r="P87" s="4"/>
       <c r="Q87" s="4"/>
@@ -7140,19 +7131,19 @@
     </row>
     <row x14ac:dyDescent="0.25" r="88" customHeight="1" ht="18.75">
       <c r="A88" s="4"/>
-      <c r="B88" s="69"/>
-      <c r="C88" s="69"/>
-      <c r="D88" s="70"/>
-      <c r="E88" s="69"/>
-      <c r="F88" s="70"/>
-      <c r="G88" s="69"/>
-      <c r="H88" s="70"/>
-      <c r="I88" s="70"/>
-      <c r="J88" s="70"/>
-      <c r="K88" s="70"/>
-      <c r="L88" s="70"/>
-      <c r="M88" s="70"/>
-      <c r="N88" s="70"/>
+      <c r="B88" s="70"/>
+      <c r="C88" s="70"/>
+      <c r="D88" s="71"/>
+      <c r="E88" s="70"/>
+      <c r="F88" s="71"/>
+      <c r="G88" s="70"/>
+      <c r="H88" s="71"/>
+      <c r="I88" s="71"/>
+      <c r="J88" s="71"/>
+      <c r="K88" s="71"/>
+      <c r="L88" s="71"/>
+      <c r="M88" s="71"/>
+      <c r="N88" s="71"/>
       <c r="O88" s="4"/>
       <c r="P88" s="4"/>
       <c r="Q88" s="4"/>
@@ -7186,19 +7177,19 @@
     </row>
     <row x14ac:dyDescent="0.25" r="89" customHeight="1" ht="18.75">
       <c r="A89" s="4"/>
-      <c r="B89" s="69"/>
-      <c r="C89" s="69"/>
-      <c r="D89" s="70"/>
-      <c r="E89" s="69"/>
-      <c r="F89" s="70"/>
-      <c r="G89" s="69"/>
-      <c r="H89" s="70"/>
-      <c r="I89" s="70"/>
-      <c r="J89" s="70"/>
-      <c r="K89" s="70"/>
-      <c r="L89" s="70"/>
-      <c r="M89" s="70"/>
-      <c r="N89" s="70"/>
+      <c r="B89" s="70"/>
+      <c r="C89" s="70"/>
+      <c r="D89" s="71"/>
+      <c r="E89" s="70"/>
+      <c r="F89" s="71"/>
+      <c r="G89" s="70"/>
+      <c r="H89" s="71"/>
+      <c r="I89" s="71"/>
+      <c r="J89" s="71"/>
+      <c r="K89" s="71"/>
+      <c r="L89" s="71"/>
+      <c r="M89" s="71"/>
+      <c r="N89" s="71"/>
       <c r="O89" s="4"/>
       <c r="P89" s="4"/>
       <c r="Q89" s="4"/>
@@ -7232,19 +7223,19 @@
     </row>
     <row x14ac:dyDescent="0.25" r="90" customHeight="1" ht="18.75">
       <c r="A90" s="4"/>
-      <c r="B90" s="69"/>
-      <c r="C90" s="69"/>
-      <c r="D90" s="70"/>
-      <c r="E90" s="69"/>
-      <c r="F90" s="70"/>
-      <c r="G90" s="69"/>
-      <c r="H90" s="70"/>
-      <c r="I90" s="70"/>
-      <c r="J90" s="70"/>
-      <c r="K90" s="70"/>
-      <c r="L90" s="70"/>
-      <c r="M90" s="70"/>
-      <c r="N90" s="70"/>
+      <c r="B90" s="70"/>
+      <c r="C90" s="70"/>
+      <c r="D90" s="71"/>
+      <c r="E90" s="70"/>
+      <c r="F90" s="71"/>
+      <c r="G90" s="70"/>
+      <c r="H90" s="71"/>
+      <c r="I90" s="71"/>
+      <c r="J90" s="71"/>
+      <c r="K90" s="71"/>
+      <c r="L90" s="71"/>
+      <c r="M90" s="71"/>
+      <c r="N90" s="71"/>
       <c r="O90" s="4"/>
       <c r="P90" s="4"/>
       <c r="Q90" s="4"/>
@@ -7278,19 +7269,19 @@
     </row>
     <row x14ac:dyDescent="0.25" r="91" customHeight="1" ht="18.75">
       <c r="A91" s="4"/>
-      <c r="B91" s="69"/>
-      <c r="C91" s="69"/>
-      <c r="D91" s="70"/>
-      <c r="E91" s="69"/>
-      <c r="F91" s="70"/>
-      <c r="G91" s="69"/>
-      <c r="H91" s="70"/>
-      <c r="I91" s="70"/>
-      <c r="J91" s="70"/>
-      <c r="K91" s="70"/>
-      <c r="L91" s="70"/>
-      <c r="M91" s="70"/>
-      <c r="N91" s="70"/>
+      <c r="B91" s="70"/>
+      <c r="C91" s="70"/>
+      <c r="D91" s="71"/>
+      <c r="E91" s="70"/>
+      <c r="F91" s="71"/>
+      <c r="G91" s="70"/>
+      <c r="H91" s="71"/>
+      <c r="I91" s="71"/>
+      <c r="J91" s="71"/>
+      <c r="K91" s="71"/>
+      <c r="L91" s="71"/>
+      <c r="M91" s="71"/>
+      <c r="N91" s="71"/>
       <c r="O91" s="4"/>
       <c r="P91" s="4"/>
       <c r="Q91" s="4"/>
@@ -7324,19 +7315,19 @@
     </row>
     <row x14ac:dyDescent="0.25" r="92" customHeight="1" ht="18.75">
       <c r="A92" s="4"/>
-      <c r="B92" s="69"/>
-      <c r="C92" s="69"/>
-      <c r="D92" s="70"/>
-      <c r="E92" s="69"/>
-      <c r="F92" s="70"/>
-      <c r="G92" s="69"/>
-      <c r="H92" s="70"/>
-      <c r="I92" s="70"/>
-      <c r="J92" s="70"/>
-      <c r="K92" s="70"/>
-      <c r="L92" s="70"/>
-      <c r="M92" s="70"/>
-      <c r="N92" s="70"/>
+      <c r="B92" s="70"/>
+      <c r="C92" s="70"/>
+      <c r="D92" s="71"/>
+      <c r="E92" s="70"/>
+      <c r="F92" s="71"/>
+      <c r="G92" s="70"/>
+      <c r="H92" s="71"/>
+      <c r="I92" s="71"/>
+      <c r="J92" s="71"/>
+      <c r="K92" s="71"/>
+      <c r="L92" s="71"/>
+      <c r="M92" s="71"/>
+      <c r="N92" s="71"/>
       <c r="O92" s="4"/>
       <c r="P92" s="4"/>
       <c r="Q92" s="4"/>
@@ -7370,19 +7361,19 @@
     </row>
     <row x14ac:dyDescent="0.25" r="93" customHeight="1" ht="18.75">
       <c r="A93" s="4"/>
-      <c r="B93" s="69"/>
-      <c r="C93" s="69"/>
-      <c r="D93" s="70"/>
-      <c r="E93" s="69"/>
-      <c r="F93" s="70"/>
-      <c r="G93" s="69"/>
-      <c r="H93" s="70"/>
-      <c r="I93" s="70"/>
-      <c r="J93" s="70"/>
-      <c r="K93" s="70"/>
-      <c r="L93" s="70"/>
-      <c r="M93" s="70"/>
-      <c r="N93" s="70"/>
+      <c r="B93" s="70"/>
+      <c r="C93" s="70"/>
+      <c r="D93" s="71"/>
+      <c r="E93" s="70"/>
+      <c r="F93" s="71"/>
+      <c r="G93" s="70"/>
+      <c r="H93" s="71"/>
+      <c r="I93" s="71"/>
+      <c r="J93" s="71"/>
+      <c r="K93" s="71"/>
+      <c r="L93" s="71"/>
+      <c r="M93" s="71"/>
+      <c r="N93" s="71"/>
       <c r="O93" s="4"/>
       <c r="P93" s="4"/>
       <c r="Q93" s="4"/>
@@ -7416,19 +7407,19 @@
     </row>
     <row x14ac:dyDescent="0.25" r="94" customHeight="1" ht="18.75">
       <c r="A94" s="4"/>
-      <c r="B94" s="69"/>
-      <c r="C94" s="69"/>
-      <c r="D94" s="70"/>
-      <c r="E94" s="69"/>
-      <c r="F94" s="70"/>
-      <c r="G94" s="69"/>
-      <c r="H94" s="70"/>
-      <c r="I94" s="70"/>
-      <c r="J94" s="70"/>
-      <c r="K94" s="70"/>
-      <c r="L94" s="70"/>
-      <c r="M94" s="70"/>
-      <c r="N94" s="70"/>
+      <c r="B94" s="70"/>
+      <c r="C94" s="70"/>
+      <c r="D94" s="71"/>
+      <c r="E94" s="70"/>
+      <c r="F94" s="71"/>
+      <c r="G94" s="70"/>
+      <c r="H94" s="71"/>
+      <c r="I94" s="71"/>
+      <c r="J94" s="71"/>
+      <c r="K94" s="71"/>
+      <c r="L94" s="71"/>
+      <c r="M94" s="71"/>
+      <c r="N94" s="71"/>
       <c r="O94" s="4"/>
       <c r="P94" s="4"/>
       <c r="Q94" s="4"/>
@@ -7462,19 +7453,19 @@
     </row>
     <row x14ac:dyDescent="0.25" r="95" customHeight="1" ht="18.75">
       <c r="A95" s="4"/>
-      <c r="B95" s="69"/>
-      <c r="C95" s="69"/>
-      <c r="D95" s="70"/>
-      <c r="E95" s="69"/>
-      <c r="F95" s="70"/>
-      <c r="G95" s="69"/>
-      <c r="H95" s="70"/>
-      <c r="I95" s="70"/>
-      <c r="J95" s="70"/>
-      <c r="K95" s="70"/>
-      <c r="L95" s="70"/>
-      <c r="M95" s="70"/>
-      <c r="N95" s="70"/>
+      <c r="B95" s="70"/>
+      <c r="C95" s="70"/>
+      <c r="D95" s="71"/>
+      <c r="E95" s="70"/>
+      <c r="F95" s="71"/>
+      <c r="G95" s="70"/>
+      <c r="H95" s="71"/>
+      <c r="I95" s="71"/>
+      <c r="J95" s="71"/>
+      <c r="K95" s="71"/>
+      <c r="L95" s="71"/>
+      <c r="M95" s="71"/>
+      <c r="N95" s="71"/>
       <c r="O95" s="4"/>
       <c r="P95" s="4"/>
       <c r="Q95" s="4"/>
@@ -7508,19 +7499,19 @@
     </row>
     <row x14ac:dyDescent="0.25" r="96" customHeight="1" ht="18.75">
       <c r="A96" s="4"/>
-      <c r="B96" s="69"/>
-      <c r="C96" s="69"/>
-      <c r="D96" s="70"/>
-      <c r="E96" s="69"/>
-      <c r="F96" s="70"/>
-      <c r="G96" s="69"/>
-      <c r="H96" s="70"/>
-      <c r="I96" s="70"/>
-      <c r="J96" s="70"/>
-      <c r="K96" s="70"/>
-      <c r="L96" s="70"/>
-      <c r="M96" s="70"/>
-      <c r="N96" s="70"/>
+      <c r="B96" s="70"/>
+      <c r="C96" s="70"/>
+      <c r="D96" s="71"/>
+      <c r="E96" s="70"/>
+      <c r="F96" s="71"/>
+      <c r="G96" s="70"/>
+      <c r="H96" s="71"/>
+      <c r="I96" s="71"/>
+      <c r="J96" s="71"/>
+      <c r="K96" s="71"/>
+      <c r="L96" s="71"/>
+      <c r="M96" s="71"/>
+      <c r="N96" s="71"/>
       <c r="O96" s="4"/>
       <c r="P96" s="4"/>
       <c r="Q96" s="4"/>
@@ -7554,19 +7545,19 @@
     </row>
     <row x14ac:dyDescent="0.25" r="97" customHeight="1" ht="18.75">
       <c r="A97" s="4"/>
-      <c r="B97" s="69"/>
-      <c r="C97" s="69"/>
-      <c r="D97" s="70"/>
-      <c r="E97" s="69"/>
-      <c r="F97" s="70"/>
-      <c r="G97" s="69"/>
-      <c r="H97" s="70"/>
-      <c r="I97" s="70"/>
-      <c r="J97" s="70"/>
-      <c r="K97" s="70"/>
-      <c r="L97" s="70"/>
-      <c r="M97" s="70"/>
-      <c r="N97" s="70"/>
+      <c r="B97" s="70"/>
+      <c r="C97" s="70"/>
+      <c r="D97" s="71"/>
+      <c r="E97" s="70"/>
+      <c r="F97" s="71"/>
+      <c r="G97" s="70"/>
+      <c r="H97" s="71"/>
+      <c r="I97" s="71"/>
+      <c r="J97" s="71"/>
+      <c r="K97" s="71"/>
+      <c r="L97" s="71"/>
+      <c r="M97" s="71"/>
+      <c r="N97" s="71"/>
       <c r="O97" s="4"/>
       <c r="P97" s="4"/>
       <c r="Q97" s="4"/>
@@ -7600,19 +7591,19 @@
     </row>
     <row x14ac:dyDescent="0.25" r="98" customHeight="1" ht="18.75">
       <c r="A98" s="4"/>
-      <c r="B98" s="69"/>
-      <c r="C98" s="69"/>
-      <c r="D98" s="70"/>
-      <c r="E98" s="69"/>
-      <c r="F98" s="70"/>
-      <c r="G98" s="69"/>
-      <c r="H98" s="70"/>
-      <c r="I98" s="70"/>
-      <c r="J98" s="70"/>
-      <c r="K98" s="70"/>
-      <c r="L98" s="70"/>
-      <c r="M98" s="70"/>
-      <c r="N98" s="70"/>
+      <c r="B98" s="70"/>
+      <c r="C98" s="70"/>
+      <c r="D98" s="71"/>
+      <c r="E98" s="70"/>
+      <c r="F98" s="71"/>
+      <c r="G98" s="70"/>
+      <c r="H98" s="71"/>
+      <c r="I98" s="71"/>
+      <c r="J98" s="71"/>
+      <c r="K98" s="71"/>
+      <c r="L98" s="71"/>
+      <c r="M98" s="71"/>
+      <c r="N98" s="71"/>
       <c r="O98" s="4"/>
       <c r="P98" s="4"/>
       <c r="Q98" s="4"/>
@@ -7646,19 +7637,19 @@
     </row>
     <row x14ac:dyDescent="0.25" r="99" customHeight="1" ht="18.75">
       <c r="A99" s="4"/>
-      <c r="B99" s="69"/>
-      <c r="C99" s="69"/>
-      <c r="D99" s="70"/>
-      <c r="E99" s="69"/>
-      <c r="F99" s="70"/>
-      <c r="G99" s="69"/>
-      <c r="H99" s="70"/>
-      <c r="I99" s="70"/>
-      <c r="J99" s="70"/>
-      <c r="K99" s="70"/>
-      <c r="L99" s="70"/>
-      <c r="M99" s="70"/>
-      <c r="N99" s="70"/>
+      <c r="B99" s="70"/>
+      <c r="C99" s="70"/>
+      <c r="D99" s="71"/>
+      <c r="E99" s="70"/>
+      <c r="F99" s="71"/>
+      <c r="G99" s="70"/>
+      <c r="H99" s="71"/>
+      <c r="I99" s="71"/>
+      <c r="J99" s="71"/>
+      <c r="K99" s="71"/>
+      <c r="L99" s="71"/>
+      <c r="M99" s="71"/>
+      <c r="N99" s="71"/>
       <c r="O99" s="4"/>
       <c r="P99" s="4"/>
       <c r="Q99" s="4"/>
@@ -7692,19 +7683,19 @@
     </row>
     <row x14ac:dyDescent="0.25" r="100" customHeight="1" ht="18.75">
       <c r="A100" s="4"/>
-      <c r="B100" s="69"/>
-      <c r="C100" s="69"/>
-      <c r="D100" s="70"/>
-      <c r="E100" s="69"/>
-      <c r="F100" s="70"/>
-      <c r="G100" s="69"/>
-      <c r="H100" s="70"/>
-      <c r="I100" s="70"/>
-      <c r="J100" s="70"/>
-      <c r="K100" s="70"/>
-      <c r="L100" s="70"/>
-      <c r="M100" s="70"/>
-      <c r="N100" s="70"/>
+      <c r="B100" s="70"/>
+      <c r="C100" s="70"/>
+      <c r="D100" s="71"/>
+      <c r="E100" s="70"/>
+      <c r="F100" s="71"/>
+      <c r="G100" s="70"/>
+      <c r="H100" s="71"/>
+      <c r="I100" s="71"/>
+      <c r="J100" s="71"/>
+      <c r="K100" s="71"/>
+      <c r="L100" s="71"/>
+      <c r="M100" s="71"/>
+      <c r="N100" s="71"/>
       <c r="O100" s="4"/>
       <c r="P100" s="4"/>
       <c r="Q100" s="4"/>
@@ -7738,19 +7729,19 @@
     </row>
     <row x14ac:dyDescent="0.25" r="101" customHeight="1" ht="18.75">
       <c r="A101" s="4"/>
-      <c r="B101" s="69"/>
-      <c r="C101" s="69"/>
-      <c r="D101" s="70"/>
-      <c r="E101" s="69"/>
-      <c r="F101" s="70"/>
-      <c r="G101" s="69"/>
-      <c r="H101" s="70"/>
-      <c r="I101" s="70"/>
-      <c r="J101" s="70"/>
-      <c r="K101" s="70"/>
-      <c r="L101" s="70"/>
-      <c r="M101" s="70"/>
-      <c r="N101" s="70"/>
+      <c r="B101" s="70"/>
+      <c r="C101" s="70"/>
+      <c r="D101" s="71"/>
+      <c r="E101" s="70"/>
+      <c r="F101" s="71"/>
+      <c r="G101" s="70"/>
+      <c r="H101" s="71"/>
+      <c r="I101" s="71"/>
+      <c r="J101" s="71"/>
+      <c r="K101" s="71"/>
+      <c r="L101" s="71"/>
+      <c r="M101" s="71"/>
+      <c r="N101" s="71"/>
       <c r="O101" s="4"/>
       <c r="P101" s="4"/>
       <c r="Q101" s="4"/>
@@ -7784,19 +7775,19 @@
     </row>
     <row x14ac:dyDescent="0.25" r="102" customHeight="1" ht="18.75">
       <c r="A102" s="4"/>
-      <c r="B102" s="69"/>
-      <c r="C102" s="69"/>
-      <c r="D102" s="70"/>
-      <c r="E102" s="69"/>
-      <c r="F102" s="70"/>
-      <c r="G102" s="69"/>
-      <c r="H102" s="70"/>
-      <c r="I102" s="70"/>
-      <c r="J102" s="70"/>
-      <c r="K102" s="70"/>
-      <c r="L102" s="70"/>
-      <c r="M102" s="70"/>
-      <c r="N102" s="70"/>
+      <c r="B102" s="70"/>
+      <c r="C102" s="70"/>
+      <c r="D102" s="71"/>
+      <c r="E102" s="70"/>
+      <c r="F102" s="71"/>
+      <c r="G102" s="70"/>
+      <c r="H102" s="71"/>
+      <c r="I102" s="71"/>
+      <c r="J102" s="71"/>
+      <c r="K102" s="71"/>
+      <c r="L102" s="71"/>
+      <c r="M102" s="71"/>
+      <c r="N102" s="71"/>
       <c r="O102" s="4"/>
       <c r="P102" s="4"/>
       <c r="Q102" s="4"/>
@@ -7830,19 +7821,19 @@
     </row>
     <row x14ac:dyDescent="0.25" r="103" customHeight="1" ht="18.75">
       <c r="A103" s="4"/>
-      <c r="B103" s="69"/>
-      <c r="C103" s="69"/>
-      <c r="D103" s="70"/>
-      <c r="E103" s="69"/>
-      <c r="F103" s="70"/>
-      <c r="G103" s="69"/>
-      <c r="H103" s="70"/>
-      <c r="I103" s="70"/>
-      <c r="J103" s="70"/>
-      <c r="K103" s="70"/>
-      <c r="L103" s="70"/>
-      <c r="M103" s="70"/>
-      <c r="N103" s="70"/>
+      <c r="B103" s="70"/>
+      <c r="C103" s="70"/>
+      <c r="D103" s="71"/>
+      <c r="E103" s="70"/>
+      <c r="F103" s="71"/>
+      <c r="G103" s="70"/>
+      <c r="H103" s="71"/>
+      <c r="I103" s="71"/>
+      <c r="J103" s="71"/>
+      <c r="K103" s="71"/>
+      <c r="L103" s="71"/>
+      <c r="M103" s="71"/>
+      <c r="N103" s="71"/>
       <c r="O103" s="4"/>
       <c r="P103" s="4"/>
       <c r="Q103" s="4"/>
@@ -7876,19 +7867,19 @@
     </row>
     <row x14ac:dyDescent="0.25" r="104" customHeight="1" ht="18.75">
       <c r="A104" s="4"/>
-      <c r="B104" s="69"/>
-      <c r="C104" s="69"/>
-      <c r="D104" s="70"/>
-      <c r="E104" s="69"/>
-      <c r="F104" s="70"/>
-      <c r="G104" s="69"/>
-      <c r="H104" s="70"/>
-      <c r="I104" s="70"/>
-      <c r="J104" s="70"/>
-      <c r="K104" s="70"/>
-      <c r="L104" s="70"/>
-      <c r="M104" s="70"/>
-      <c r="N104" s="70"/>
+      <c r="B104" s="70"/>
+      <c r="C104" s="70"/>
+      <c r="D104" s="71"/>
+      <c r="E104" s="70"/>
+      <c r="F104" s="71"/>
+      <c r="G104" s="70"/>
+      <c r="H104" s="71"/>
+      <c r="I104" s="71"/>
+      <c r="J104" s="71"/>
+      <c r="K104" s="71"/>
+      <c r="L104" s="71"/>
+      <c r="M104" s="71"/>
+      <c r="N104" s="71"/>
       <c r="O104" s="4"/>
       <c r="P104" s="4"/>
       <c r="Q104" s="4"/>
@@ -7922,19 +7913,19 @@
     </row>
     <row x14ac:dyDescent="0.25" r="105" customHeight="1" ht="18.75">
       <c r="A105" s="4"/>
-      <c r="B105" s="69"/>
-      <c r="C105" s="69"/>
-      <c r="D105" s="70"/>
-      <c r="E105" s="69"/>
-      <c r="F105" s="70"/>
-      <c r="G105" s="69"/>
-      <c r="H105" s="70"/>
-      <c r="I105" s="70"/>
-      <c r="J105" s="70"/>
-      <c r="K105" s="70"/>
-      <c r="L105" s="70"/>
-      <c r="M105" s="70"/>
-      <c r="N105" s="70"/>
+      <c r="B105" s="70"/>
+      <c r="C105" s="70"/>
+      <c r="D105" s="71"/>
+      <c r="E105" s="70"/>
+      <c r="F105" s="71"/>
+      <c r="G105" s="70"/>
+      <c r="H105" s="71"/>
+      <c r="I105" s="71"/>
+      <c r="J105" s="71"/>
+      <c r="K105" s="71"/>
+      <c r="L105" s="71"/>
+      <c r="M105" s="71"/>
+      <c r="N105" s="71"/>
       <c r="O105" s="4"/>
       <c r="P105" s="4"/>
       <c r="Q105" s="4"/>
@@ -7968,19 +7959,19 @@
     </row>
     <row x14ac:dyDescent="0.25" r="106" customHeight="1" ht="18.75">
       <c r="A106" s="4"/>
-      <c r="B106" s="69"/>
-      <c r="C106" s="69"/>
-      <c r="D106" s="70"/>
-      <c r="E106" s="69"/>
-      <c r="F106" s="70"/>
-      <c r="G106" s="69"/>
-      <c r="H106" s="70"/>
-      <c r="I106" s="70"/>
-      <c r="J106" s="70"/>
-      <c r="K106" s="70"/>
-      <c r="L106" s="70"/>
-      <c r="M106" s="70"/>
-      <c r="N106" s="70"/>
+      <c r="B106" s="70"/>
+      <c r="C106" s="70"/>
+      <c r="D106" s="71"/>
+      <c r="E106" s="70"/>
+      <c r="F106" s="71"/>
+      <c r="G106" s="70"/>
+      <c r="H106" s="71"/>
+      <c r="I106" s="71"/>
+      <c r="J106" s="71"/>
+      <c r="K106" s="71"/>
+      <c r="L106" s="71"/>
+      <c r="M106" s="71"/>
+      <c r="N106" s="71"/>
       <c r="O106" s="4"/>
       <c r="P106" s="4"/>
       <c r="Q106" s="4"/>
@@ -8014,19 +8005,19 @@
     </row>
     <row x14ac:dyDescent="0.25" r="107" customHeight="1" ht="18.75">
       <c r="A107" s="4"/>
-      <c r="B107" s="69"/>
-      <c r="C107" s="69"/>
-      <c r="D107" s="70"/>
-      <c r="E107" s="69"/>
-      <c r="F107" s="70"/>
-      <c r="G107" s="69"/>
-      <c r="H107" s="70"/>
-      <c r="I107" s="70"/>
-      <c r="J107" s="70"/>
-      <c r="K107" s="70"/>
-      <c r="L107" s="70"/>
-      <c r="M107" s="70"/>
-      <c r="N107" s="70"/>
+      <c r="B107" s="70"/>
+      <c r="C107" s="70"/>
+      <c r="D107" s="71"/>
+      <c r="E107" s="70"/>
+      <c r="F107" s="71"/>
+      <c r="G107" s="70"/>
+      <c r="H107" s="71"/>
+      <c r="I107" s="71"/>
+      <c r="J107" s="71"/>
+      <c r="K107" s="71"/>
+      <c r="L107" s="71"/>
+      <c r="M107" s="71"/>
+      <c r="N107" s="71"/>
       <c r="O107" s="4"/>
       <c r="P107" s="4"/>
       <c r="Q107" s="4"/>
@@ -8060,19 +8051,19 @@
     </row>
     <row x14ac:dyDescent="0.25" r="108" customHeight="1" ht="18.75">
       <c r="A108" s="4"/>
-      <c r="B108" s="69"/>
-      <c r="C108" s="69"/>
-      <c r="D108" s="70"/>
-      <c r="E108" s="69"/>
-      <c r="F108" s="70"/>
-      <c r="G108" s="69"/>
-      <c r="H108" s="70"/>
-      <c r="I108" s="70"/>
-      <c r="J108" s="70"/>
-      <c r="K108" s="70"/>
-      <c r="L108" s="70"/>
-      <c r="M108" s="70"/>
-      <c r="N108" s="70"/>
+      <c r="B108" s="70"/>
+      <c r="C108" s="70"/>
+      <c r="D108" s="71"/>
+      <c r="E108" s="70"/>
+      <c r="F108" s="71"/>
+      <c r="G108" s="70"/>
+      <c r="H108" s="71"/>
+      <c r="I108" s="71"/>
+      <c r="J108" s="71"/>
+      <c r="K108" s="71"/>
+      <c r="L108" s="71"/>
+      <c r="M108" s="71"/>
+      <c r="N108" s="71"/>
       <c r="O108" s="4"/>
       <c r="P108" s="4"/>
       <c r="Q108" s="4"/>
@@ -8106,19 +8097,19 @@
     </row>
     <row x14ac:dyDescent="0.25" r="109" customHeight="1" ht="18.75">
       <c r="A109" s="4"/>
-      <c r="B109" s="69"/>
-      <c r="C109" s="69"/>
-      <c r="D109" s="70"/>
-      <c r="E109" s="69"/>
-      <c r="F109" s="70"/>
-      <c r="G109" s="69"/>
-      <c r="H109" s="70"/>
-      <c r="I109" s="70"/>
-      <c r="J109" s="70"/>
-      <c r="K109" s="70"/>
-      <c r="L109" s="70"/>
-      <c r="M109" s="70"/>
-      <c r="N109" s="70"/>
+      <c r="B109" s="70"/>
+      <c r="C109" s="70"/>
+      <c r="D109" s="71"/>
+      <c r="E109" s="70"/>
+      <c r="F109" s="71"/>
+      <c r="G109" s="70"/>
+      <c r="H109" s="71"/>
+      <c r="I109" s="71"/>
+      <c r="J109" s="71"/>
+      <c r="K109" s="71"/>
+      <c r="L109" s="71"/>
+      <c r="M109" s="71"/>
+      <c r="N109" s="71"/>
       <c r="O109" s="4"/>
       <c r="P109" s="4"/>
       <c r="Q109" s="4"/>
@@ -8152,19 +8143,19 @@
     </row>
     <row x14ac:dyDescent="0.25" r="110" customHeight="1" ht="18.75">
       <c r="A110" s="4"/>
-      <c r="B110" s="69"/>
-      <c r="C110" s="69"/>
-      <c r="D110" s="70"/>
-      <c r="E110" s="69"/>
-      <c r="F110" s="70"/>
-      <c r="G110" s="69"/>
-      <c r="H110" s="70"/>
-      <c r="I110" s="70"/>
-      <c r="J110" s="70"/>
-      <c r="K110" s="70"/>
-      <c r="L110" s="70"/>
-      <c r="M110" s="70"/>
-      <c r="N110" s="70"/>
+      <c r="B110" s="70"/>
+      <c r="C110" s="70"/>
+      <c r="D110" s="71"/>
+      <c r="E110" s="70"/>
+      <c r="F110" s="71"/>
+      <c r="G110" s="70"/>
+      <c r="H110" s="71"/>
+      <c r="I110" s="71"/>
+      <c r="J110" s="71"/>
+      <c r="K110" s="71"/>
+      <c r="L110" s="71"/>
+      <c r="M110" s="71"/>
+      <c r="N110" s="71"/>
       <c r="O110" s="4"/>
       <c r="P110" s="4"/>
       <c r="Q110" s="4"/>
@@ -8198,19 +8189,19 @@
     </row>
     <row x14ac:dyDescent="0.25" r="111" customHeight="1" ht="18.75">
       <c r="A111" s="4"/>
-      <c r="B111" s="69"/>
-      <c r="C111" s="69"/>
-      <c r="D111" s="70"/>
-      <c r="E111" s="69"/>
-      <c r="F111" s="70"/>
-      <c r="G111" s="69"/>
-      <c r="H111" s="70"/>
-      <c r="I111" s="70"/>
-      <c r="J111" s="70"/>
-      <c r="K111" s="70"/>
-      <c r="L111" s="70"/>
-      <c r="M111" s="70"/>
-      <c r="N111" s="70"/>
+      <c r="B111" s="70"/>
+      <c r="C111" s="70"/>
+      <c r="D111" s="71"/>
+      <c r="E111" s="70"/>
+      <c r="F111" s="71"/>
+      <c r="G111" s="70"/>
+      <c r="H111" s="71"/>
+      <c r="I111" s="71"/>
+      <c r="J111" s="71"/>
+      <c r="K111" s="71"/>
+      <c r="L111" s="71"/>
+      <c r="M111" s="71"/>
+      <c r="N111" s="71"/>
       <c r="O111" s="4"/>
       <c r="P111" s="4"/>
       <c r="Q111" s="4"/>
@@ -8364,63 +8355,65 @@
   </sheetPr>
   <dimension ref="A1:AF71"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="41" width="15.719285714285713" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="41" width="15.719285714285713" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="39" width="24.290714285714284" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="40" width="15.719285714285713" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="40" width="15.719285714285713" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="40" width="15.719285714285713" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="40" width="15.719285714285713" customWidth="1" bestFit="1"/>
-    <col min="8" max="8" style="40" width="15.719285714285713" customWidth="1" bestFit="1"/>
-    <col min="9" max="9" style="40" width="15.719285714285713" customWidth="1" bestFit="1"/>
-    <col min="10" max="10" style="39" width="15.719285714285713" customWidth="1" bestFit="1"/>
-    <col min="11" max="11" style="40" width="15.719285714285713" customWidth="1" bestFit="1"/>
-    <col min="12" max="12" style="40" width="15.719285714285713" customWidth="1" bestFit="1"/>
-    <col min="13" max="13" style="40" width="15.719285714285713" customWidth="1" bestFit="1"/>
-    <col min="14" max="14" style="40" width="15.719285714285713" customWidth="1" bestFit="1"/>
-    <col min="15" max="15" style="40" width="15.719285714285713" customWidth="1" bestFit="1"/>
-    <col min="16" max="16" style="41" width="15.719285714285713" customWidth="1" bestFit="1"/>
-    <col min="17" max="17" style="41" width="64.005" customWidth="1" bestFit="1"/>
-    <col min="18" max="18" style="41" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="19" max="19" style="41" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="20" max="20" style="41" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="21" max="21" style="41" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="22" max="22" style="41" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="23" max="23" style="41" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="24" max="24" style="41" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="25" max="25" style="41" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="26" max="26" style="41" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="27" max="27" style="41" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="28" max="28" style="41" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="29" max="29" style="41" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="30" max="30" style="41" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="31" max="31" style="41" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="32" max="32" style="41" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="40" width="15.719285714285713" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="40" width="15.719285714285713" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="38" width="24.290714285714284" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="39" width="15.719285714285713" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="39" width="15.719285714285713" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="39" width="15.719285714285713" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="39" width="15.719285714285713" customWidth="1" bestFit="1"/>
+    <col min="8" max="8" style="39" width="15.719285714285713" customWidth="1" bestFit="1"/>
+    <col min="9" max="9" style="39" width="15.719285714285713" customWidth="1" bestFit="1"/>
+    <col min="10" max="10" style="38" width="15.719285714285713" customWidth="1" bestFit="1"/>
+    <col min="11" max="11" style="39" width="15.719285714285713" customWidth="1" bestFit="1"/>
+    <col min="12" max="12" style="39" width="15.719285714285713" customWidth="1" bestFit="1"/>
+    <col min="13" max="13" style="39" width="15.719285714285713" customWidth="1" bestFit="1"/>
+    <col min="14" max="14" style="39" width="15.719285714285713" customWidth="1" bestFit="1"/>
+    <col min="15" max="15" style="39" width="15.719285714285713" customWidth="1" bestFit="1"/>
+    <col min="16" max="16" style="40" width="15.719285714285713" customWidth="1" bestFit="1"/>
+    <col min="17" max="17" style="69" width="64.005" customWidth="1" bestFit="1"/>
+    <col min="18" max="18" style="69" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="19" max="19" style="40" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="20" max="20" style="40" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="21" max="21" style="40" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="22" max="22" style="40" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="23" max="23" style="40" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="24" max="24" style="40" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="25" max="25" style="40" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="26" max="26" style="40" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="27" max="27" style="40" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="28" max="28" style="40" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="29" max="29" style="40" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="30" max="30" style="40" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="31" max="31" style="40" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="32" max="32" style="40" width="13.576428571428572" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
-      <c r="A1" s="4"/>
+      <c r="A1" s="4" t="s">
+        <v>26</v>
+      </c>
       <c r="B1" s="4"/>
-      <c r="C1" s="42"/>
-      <c r="D1" s="43"/>
-      <c r="E1" s="43"/>
-      <c r="F1" s="43"/>
-      <c r="G1" s="43"/>
-      <c r="H1" s="43"/>
-      <c r="I1" s="43"/>
-      <c r="J1" s="42"/>
-      <c r="K1" s="43"/>
-      <c r="L1" s="43"/>
-      <c r="M1" s="43"/>
-      <c r="N1" s="43"/>
-      <c r="O1" s="43"/>
+      <c r="C1" s="41"/>
+      <c r="D1" s="42"/>
+      <c r="E1" s="42"/>
+      <c r="F1" s="42"/>
+      <c r="G1" s="42"/>
+      <c r="H1" s="42"/>
+      <c r="I1" s="42"/>
+      <c r="J1" s="41"/>
+      <c r="K1" s="42"/>
+      <c r="L1" s="42"/>
+      <c r="M1" s="42"/>
+      <c r="N1" s="42"/>
+      <c r="O1" s="42"/>
       <c r="P1" s="4"/>
-      <c r="Q1" s="4"/>
-      <c r="R1" s="4"/>
+      <c r="Q1" s="43"/>
+      <c r="R1" s="43"/>
       <c r="S1" s="4"/>
       <c r="T1" s="4"/>
       <c r="U1" s="4"/>
@@ -8439,22 +8432,22 @@
     <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
       <c r="A2" s="4"/>
       <c r="B2" s="4"/>
-      <c r="C2" s="42"/>
-      <c r="D2" s="43"/>
-      <c r="E2" s="43"/>
-      <c r="F2" s="43"/>
-      <c r="G2" s="43"/>
-      <c r="H2" s="43"/>
-      <c r="I2" s="43"/>
-      <c r="J2" s="42"/>
-      <c r="K2" s="43"/>
-      <c r="L2" s="43"/>
-      <c r="M2" s="43"/>
-      <c r="N2" s="43"/>
-      <c r="O2" s="43"/>
+      <c r="C2" s="41"/>
+      <c r="D2" s="42"/>
+      <c r="E2" s="42"/>
+      <c r="F2" s="42"/>
+      <c r="G2" s="42"/>
+      <c r="H2" s="42"/>
+      <c r="I2" s="42"/>
+      <c r="J2" s="41"/>
+      <c r="K2" s="42"/>
+      <c r="L2" s="42"/>
+      <c r="M2" s="42"/>
+      <c r="N2" s="42"/>
+      <c r="O2" s="42"/>
       <c r="P2" s="4"/>
-      <c r="Q2" s="4"/>
-      <c r="R2" s="4"/>
+      <c r="Q2" s="43"/>
+      <c r="R2" s="43"/>
       <c r="S2" s="4"/>
       <c r="T2" s="4"/>
       <c r="U2" s="4"/>
@@ -8502,7 +8495,7 @@
       <c r="Q3" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="R3" s="4"/>
+      <c r="R3" s="43"/>
       <c r="S3" s="4"/>
       <c r="T3" s="4"/>
       <c r="U3" s="4"/>
@@ -8564,7 +8557,7 @@
       <c r="Q4" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="R4" s="4"/>
+      <c r="R4" s="43"/>
       <c r="S4" s="4"/>
       <c r="T4" s="4"/>
       <c r="U4" s="4"/>
@@ -8625,8 +8618,8 @@
         <v>3.3</v>
       </c>
       <c r="P5" s="4"/>
-      <c r="Q5" s="4"/>
-      <c r="R5" s="4"/>
+      <c r="Q5" s="43"/>
+      <c r="R5" s="43"/>
       <c r="S5" s="4"/>
       <c r="T5" s="4"/>
       <c r="U5" s="4"/>
@@ -8685,8 +8678,8 @@
         <v>3.3</v>
       </c>
       <c r="P6" s="4"/>
-      <c r="Q6" s="4"/>
-      <c r="R6" s="4"/>
+      <c r="Q6" s="43"/>
+      <c r="R6" s="43"/>
       <c r="S6" s="4"/>
       <c r="T6" s="4"/>
       <c r="U6" s="4"/>
@@ -8745,8 +8738,8 @@
         <v>3.3</v>
       </c>
       <c r="P7" s="4"/>
-      <c r="Q7" s="4"/>
-      <c r="R7" s="4"/>
+      <c r="Q7" s="43"/>
+      <c r="R7" s="43"/>
       <c r="S7" s="4"/>
       <c r="T7" s="4"/>
       <c r="U7" s="4"/>
@@ -8805,8 +8798,8 @@
         <v>3.4</v>
       </c>
       <c r="P8" s="4"/>
-      <c r="Q8" s="4"/>
-      <c r="R8" s="4"/>
+      <c r="Q8" s="43"/>
+      <c r="R8" s="43"/>
       <c r="S8" s="4"/>
       <c r="T8" s="4"/>
       <c r="U8" s="4"/>
@@ -8865,8 +8858,8 @@
         <v>3</v>
       </c>
       <c r="P9" s="4"/>
-      <c r="Q9" s="4"/>
-      <c r="R9" s="4"/>
+      <c r="Q9" s="43"/>
+      <c r="R9" s="43"/>
       <c r="S9" s="4"/>
       <c r="T9" s="4"/>
       <c r="U9" s="4"/>
@@ -8925,8 +8918,8 @@
         <v>3.26</v>
       </c>
       <c r="P10" s="4"/>
-      <c r="Q10" s="4"/>
-      <c r="R10" s="4"/>
+      <c r="Q10" s="43"/>
+      <c r="R10" s="43"/>
       <c r="S10" s="4"/>
       <c r="T10" s="4"/>
       <c r="U10" s="4"/>
@@ -8959,8 +8952,8 @@
       <c r="N11" s="56"/>
       <c r="O11" s="56"/>
       <c r="P11" s="4"/>
-      <c r="Q11" s="4"/>
-      <c r="R11" s="4"/>
+      <c r="Q11" s="43"/>
+      <c r="R11" s="43"/>
       <c r="S11" s="4"/>
       <c r="T11" s="4"/>
       <c r="U11" s="4"/>
@@ -8993,8 +8986,8 @@
       <c r="N12" s="58"/>
       <c r="O12" s="58"/>
       <c r="P12" s="4"/>
-      <c r="Q12" s="4"/>
-      <c r="R12" s="4"/>
+      <c r="Q12" s="43"/>
+      <c r="R12" s="43"/>
       <c r="S12" s="4"/>
       <c r="T12" s="4"/>
       <c r="U12" s="4"/>
@@ -9027,8 +9020,8 @@
       <c r="N13" s="58"/>
       <c r="O13" s="58"/>
       <c r="P13" s="4"/>
-      <c r="Q13" s="4"/>
-      <c r="R13" s="4"/>
+      <c r="Q13" s="43"/>
+      <c r="R13" s="43"/>
       <c r="S13" s="4"/>
       <c r="T13" s="4"/>
       <c r="U13" s="4"/>
@@ -9067,8 +9060,8 @@
       <c r="N14" s="45"/>
       <c r="O14" s="45"/>
       <c r="P14" s="4"/>
-      <c r="Q14" s="4"/>
-      <c r="R14" s="4"/>
+      <c r="Q14" s="43"/>
+      <c r="R14" s="43"/>
       <c r="S14" s="4"/>
       <c r="T14" s="4"/>
       <c r="U14" s="4"/>
@@ -9121,11 +9114,11 @@
       <c r="T15" s="29"/>
       <c r="U15" s="29"/>
       <c r="V15" s="29"/>
-      <c r="W15" s="30"/>
-      <c r="X15" s="30"/>
-      <c r="Y15" s="30"/>
-      <c r="Z15" s="30"/>
-      <c r="AA15" s="30"/>
+      <c r="W15" s="29"/>
+      <c r="X15" s="29"/>
+      <c r="Y15" s="29"/>
+      <c r="Z15" s="29"/>
+      <c r="AA15" s="29"/>
       <c r="AB15" s="4"/>
       <c r="AC15" s="4"/>
       <c r="AD15" s="4"/>
@@ -9193,7 +9186,7 @@
     <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="24">
       <c r="A17" s="9"/>
       <c r="B17" s="61" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C17" s="49">
         <v>1</v>
@@ -9603,8 +9596,8 @@
       <c r="N24" s="58"/>
       <c r="O24" s="58"/>
       <c r="P24" s="4"/>
-      <c r="Q24" s="4"/>
-      <c r="R24" s="4"/>
+      <c r="Q24" s="43"/>
+      <c r="R24" s="43"/>
       <c r="S24" s="4"/>
       <c r="T24" s="4"/>
       <c r="U24" s="4"/>
@@ -9637,8 +9630,8 @@
       <c r="N25" s="58"/>
       <c r="O25" s="58"/>
       <c r="P25" s="4"/>
-      <c r="Q25" s="4"/>
-      <c r="R25" s="4"/>
+      <c r="Q25" s="43"/>
+      <c r="R25" s="43"/>
       <c r="S25" s="4"/>
       <c r="T25" s="4"/>
       <c r="U25" s="4"/>
@@ -9677,22 +9670,22 @@
       <c r="N26" s="45"/>
       <c r="O26" s="45"/>
       <c r="P26" s="4"/>
-      <c r="Q26" s="4"/>
-      <c r="R26" s="4"/>
+      <c r="Q26" s="43"/>
+      <c r="R26" s="43"/>
       <c r="S26" s="4"/>
       <c r="T26" s="4"/>
       <c r="U26" s="4"/>
       <c r="V26" s="4"/>
-      <c r="W26" s="30"/>
-      <c r="X26" s="30"/>
+      <c r="W26" s="29"/>
+      <c r="X26" s="29"/>
       <c r="Y26" s="29"/>
       <c r="Z26" s="29"/>
       <c r="AA26" s="29"/>
-      <c r="AB26" s="30"/>
-      <c r="AC26" s="30"/>
-      <c r="AD26" s="30"/>
-      <c r="AE26" s="30"/>
-      <c r="AF26" s="30"/>
+      <c r="AB26" s="29"/>
+      <c r="AC26" s="29"/>
+      <c r="AD26" s="29"/>
+      <c r="AE26" s="29"/>
+      <c r="AF26" s="29"/>
     </row>
     <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="42.6">
       <c r="A27" s="9"/>
@@ -9731,16 +9724,16 @@
       <c r="T27" s="4"/>
       <c r="U27" s="4"/>
       <c r="V27" s="4"/>
-      <c r="W27" s="30"/>
-      <c r="X27" s="30"/>
+      <c r="W27" s="29"/>
+      <c r="X27" s="29"/>
       <c r="Y27" s="29"/>
       <c r="Z27" s="29"/>
       <c r="AA27" s="29"/>
-      <c r="AB27" s="30"/>
-      <c r="AC27" s="30"/>
-      <c r="AD27" s="30"/>
-      <c r="AE27" s="30"/>
-      <c r="AF27" s="30"/>
+      <c r="AB27" s="29"/>
+      <c r="AC27" s="29"/>
+      <c r="AD27" s="29"/>
+      <c r="AE27" s="29"/>
+      <c r="AF27" s="29"/>
     </row>
     <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="18.75">
       <c r="A28" s="9"/>
@@ -9803,7 +9796,7 @@
     <row x14ac:dyDescent="0.25" r="29" customHeight="1" ht="24">
       <c r="A29" s="9"/>
       <c r="B29" s="48" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C29" s="49">
         <v>1</v>
@@ -10105,7 +10098,7 @@
     <row x14ac:dyDescent="0.25" r="34" customHeight="1" ht="18.75">
       <c r="A34" s="9"/>
       <c r="B34" s="9"/>
-      <c r="C34" s="35" t="s">
+      <c r="C34" s="34" t="s">
         <v>14</v>
       </c>
       <c r="D34" s="67">
@@ -10213,8 +10206,8 @@
       <c r="N36" s="58"/>
       <c r="O36" s="58"/>
       <c r="P36" s="4"/>
-      <c r="Q36" s="4"/>
-      <c r="R36" s="4"/>
+      <c r="Q36" s="43"/>
+      <c r="R36" s="43"/>
       <c r="S36" s="4"/>
       <c r="T36" s="4"/>
       <c r="U36" s="4"/>
@@ -10247,8 +10240,8 @@
       <c r="N37" s="58"/>
       <c r="O37" s="58"/>
       <c r="P37" s="4"/>
-      <c r="Q37" s="4"/>
-      <c r="R37" s="4"/>
+      <c r="Q37" s="43"/>
+      <c r="R37" s="43"/>
       <c r="S37" s="4"/>
       <c r="T37" s="4"/>
       <c r="U37" s="4"/>
@@ -10287,8 +10280,8 @@
       <c r="N38" s="45"/>
       <c r="O38" s="45"/>
       <c r="P38" s="4"/>
-      <c r="Q38" s="4"/>
-      <c r="R38" s="4"/>
+      <c r="Q38" s="43"/>
+      <c r="R38" s="43"/>
       <c r="S38" s="4"/>
       <c r="T38" s="4"/>
       <c r="U38" s="4"/>
@@ -10413,7 +10406,7 @@
     <row x14ac:dyDescent="0.25" r="41" customHeight="1" ht="19.15">
       <c r="A41" s="9"/>
       <c r="B41" s="48" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C41" s="49">
         <v>1</v>
@@ -10823,8 +10816,8 @@
       <c r="N48" s="58"/>
       <c r="O48" s="58"/>
       <c r="P48" s="4"/>
-      <c r="Q48" s="4"/>
-      <c r="R48" s="4"/>
+      <c r="Q48" s="43"/>
+      <c r="R48" s="43"/>
       <c r="S48" s="4"/>
       <c r="T48" s="4"/>
       <c r="U48" s="4"/>
@@ -10857,8 +10850,8 @@
       <c r="N49" s="58"/>
       <c r="O49" s="58"/>
       <c r="P49" s="4"/>
-      <c r="Q49" s="4"/>
-      <c r="R49" s="4"/>
+      <c r="Q49" s="43"/>
+      <c r="R49" s="43"/>
       <c r="S49" s="4"/>
       <c r="T49" s="4"/>
       <c r="U49" s="4"/>
@@ -10897,8 +10890,8 @@
       <c r="N50" s="45"/>
       <c r="O50" s="45"/>
       <c r="P50" s="4"/>
-      <c r="Q50" s="4"/>
-      <c r="R50" s="4"/>
+      <c r="Q50" s="43"/>
+      <c r="R50" s="43"/>
       <c r="S50" s="4"/>
       <c r="T50" s="4"/>
       <c r="U50" s="4"/>
@@ -10950,16 +10943,16 @@
       <c r="S51" s="4"/>
       <c r="T51" s="4"/>
       <c r="U51" s="4"/>
-      <c r="V51" s="30"/>
-      <c r="W51" s="30"/>
+      <c r="V51" s="29"/>
+      <c r="W51" s="29"/>
       <c r="X51" s="29"/>
       <c r="Y51" s="29"/>
       <c r="Z51" s="29"/>
-      <c r="AA51" s="30"/>
-      <c r="AB51" s="30"/>
-      <c r="AC51" s="30"/>
-      <c r="AD51" s="30"/>
-      <c r="AE51" s="30"/>
+      <c r="AA51" s="29"/>
+      <c r="AB51" s="29"/>
+      <c r="AC51" s="29"/>
+      <c r="AD51" s="29"/>
+      <c r="AE51" s="29"/>
       <c r="AF51" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="52" customHeight="1" ht="18.75">
@@ -11008,22 +11001,22 @@
       <c r="S52" s="4"/>
       <c r="T52" s="4"/>
       <c r="U52" s="4"/>
-      <c r="V52" s="30"/>
-      <c r="W52" s="30"/>
+      <c r="V52" s="29"/>
+      <c r="W52" s="29"/>
       <c r="X52" s="29"/>
       <c r="Y52" s="29"/>
       <c r="Z52" s="29"/>
-      <c r="AA52" s="30"/>
-      <c r="AB52" s="30"/>
-      <c r="AC52" s="30"/>
-      <c r="AD52" s="30"/>
-      <c r="AE52" s="30"/>
+      <c r="AA52" s="29"/>
+      <c r="AB52" s="29"/>
+      <c r="AC52" s="29"/>
+      <c r="AD52" s="29"/>
+      <c r="AE52" s="29"/>
       <c r="AF52" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="53" customHeight="1" ht="24.600000000000005">
       <c r="A53" s="9"/>
       <c r="B53" s="48" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C53" s="49">
         <v>1</v>
@@ -11433,8 +11426,8 @@
       <c r="N60" s="58"/>
       <c r="O60" s="58"/>
       <c r="P60" s="4"/>
-      <c r="Q60" s="4"/>
-      <c r="R60" s="4"/>
+      <c r="Q60" s="43"/>
+      <c r="R60" s="43"/>
       <c r="S60" s="4"/>
       <c r="T60" s="4"/>
       <c r="U60" s="4"/>
@@ -11467,8 +11460,8 @@
       <c r="N61" s="58"/>
       <c r="O61" s="58"/>
       <c r="P61" s="4"/>
-      <c r="Q61" s="4"/>
-      <c r="R61" s="4"/>
+      <c r="Q61" s="43"/>
+      <c r="R61" s="43"/>
       <c r="S61" s="4"/>
       <c r="T61" s="4"/>
       <c r="U61" s="4"/>
@@ -11507,8 +11500,8 @@
       <c r="N62" s="45"/>
       <c r="O62" s="45"/>
       <c r="P62" s="4"/>
-      <c r="Q62" s="4"/>
-      <c r="R62" s="4"/>
+      <c r="Q62" s="43"/>
+      <c r="R62" s="43"/>
       <c r="S62" s="4"/>
       <c r="T62" s="4"/>
       <c r="U62" s="4"/>
@@ -11633,7 +11626,7 @@
     <row x14ac:dyDescent="0.25" r="65" customHeight="1" ht="19.15">
       <c r="A65" s="9"/>
       <c r="B65" s="48" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C65" s="49">
         <v>1</v>
@@ -12111,38 +12104,38 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="38" width="15.719285714285713" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="39" width="15.719285714285713" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="39" width="24.290714285714284" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="40" width="15.719285714285713" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="40" width="15.719285714285713" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="40" width="15.719285714285713" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="40" width="15.719285714285713" customWidth="1" bestFit="1"/>
-    <col min="8" max="8" style="40" width="15.719285714285713" customWidth="1" bestFit="1"/>
-    <col min="9" max="9" style="40" width="15.719285714285713" customWidth="1" bestFit="1"/>
-    <col min="10" max="10" style="40" width="15.719285714285713" customWidth="1" bestFit="1"/>
-    <col min="11" max="11" style="40" width="15.719285714285713" customWidth="1" bestFit="1"/>
-    <col min="12" max="12" style="40" width="15.719285714285713" customWidth="1" bestFit="1"/>
-    <col min="13" max="13" style="40" width="15.719285714285713" customWidth="1" bestFit="1"/>
-    <col min="14" max="14" style="40" width="15.719285714285713" customWidth="1" bestFit="1"/>
-    <col min="15" max="15" style="41" width="15.719285714285713" customWidth="1" bestFit="1"/>
-    <col min="16" max="16" style="41" width="15.719285714285713" customWidth="1" bestFit="1"/>
-    <col min="17" max="17" style="41" width="58.29071428571429" customWidth="1" bestFit="1"/>
-    <col min="18" max="18" style="41" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="19" max="19" style="41" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="20" max="20" style="41" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="21" max="21" style="41" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="22" max="22" style="41" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="23" max="23" style="41" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="24" max="24" style="41" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="25" max="25" style="41" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="26" max="26" style="41" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="27" max="27" style="41" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="28" max="28" style="41" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="29" max="29" style="41" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="30" max="30" style="41" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="31" max="31" style="41" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="32" max="32" style="41" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="37" width="15.719285714285713" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="38" width="15.719285714285713" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="38" width="24.290714285714284" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="39" width="15.719285714285713" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="39" width="15.719285714285713" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="39" width="15.719285714285713" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="39" width="15.719285714285713" customWidth="1" bestFit="1"/>
+    <col min="8" max="8" style="39" width="15.719285714285713" customWidth="1" bestFit="1"/>
+    <col min="9" max="9" style="39" width="15.719285714285713" customWidth="1" bestFit="1"/>
+    <col min="10" max="10" style="39" width="15.719285714285713" customWidth="1" bestFit="1"/>
+    <col min="11" max="11" style="39" width="15.719285714285713" customWidth="1" bestFit="1"/>
+    <col min="12" max="12" style="39" width="15.719285714285713" customWidth="1" bestFit="1"/>
+    <col min="13" max="13" style="39" width="15.719285714285713" customWidth="1" bestFit="1"/>
+    <col min="14" max="14" style="39" width="15.719285714285713" customWidth="1" bestFit="1"/>
+    <col min="15" max="15" style="40" width="15.719285714285713" customWidth="1" bestFit="1"/>
+    <col min="16" max="16" style="40" width="15.719285714285713" customWidth="1" bestFit="1"/>
+    <col min="17" max="17" style="40" width="58.29071428571429" customWidth="1" bestFit="1"/>
+    <col min="18" max="18" style="40" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="19" max="19" style="40" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="20" max="20" style="40" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="21" max="21" style="40" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="22" max="22" style="40" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="23" max="23" style="40" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="24" max="24" style="40" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="25" max="25" style="40" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="26" max="26" style="40" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="27" max="27" style="40" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="28" max="28" style="40" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="29" max="29" style="40" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="30" max="30" style="40" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="31" max="31" style="40" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="32" max="32" style="40" width="13.576428571428572" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="22.5">
@@ -12912,11 +12905,11 @@
       <c r="T15" s="29"/>
       <c r="U15" s="29"/>
       <c r="V15" s="29"/>
-      <c r="W15" s="30"/>
-      <c r="X15" s="30"/>
-      <c r="Y15" s="30"/>
-      <c r="Z15" s="30"/>
-      <c r="AA15" s="30"/>
+      <c r="W15" s="29"/>
+      <c r="X15" s="29"/>
+      <c r="Y15" s="29"/>
+      <c r="Z15" s="29"/>
+      <c r="AA15" s="29"/>
       <c r="AB15" s="4"/>
       <c r="AC15" s="4"/>
       <c r="AD15" s="4"/>
@@ -12924,10 +12917,10 @@
       <c r="AF15" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="23.25">
-      <c r="A16" s="31" t="s">
+      <c r="A16" s="30" t="s">
         <v>20</v>
       </c>
-      <c r="B16" s="32">
+      <c r="B16" s="31">
         <v>1</v>
       </c>
       <c r="C16" s="17">
@@ -12986,8 +12979,8 @@
       <c r="AF16" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="23.25">
-      <c r="A17" s="33"/>
-      <c r="B17" s="32">
+      <c r="A17" s="32"/>
+      <c r="B17" s="31">
         <v>2</v>
       </c>
       <c r="C17" s="17">
@@ -13046,8 +13039,8 @@
       <c r="AF17" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="23.25">
-      <c r="A18" s="33"/>
-      <c r="B18" s="32">
+      <c r="A18" s="32"/>
+      <c r="B18" s="31">
         <v>3</v>
       </c>
       <c r="C18" s="17">
@@ -13106,8 +13099,8 @@
       <c r="AF18" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="23.25">
-      <c r="A19" s="33"/>
-      <c r="B19" s="32">
+      <c r="A19" s="32"/>
+      <c r="B19" s="31">
         <v>4</v>
       </c>
       <c r="C19" s="17">
@@ -13166,8 +13159,8 @@
       <c r="AF19" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="23.25">
-      <c r="A20" s="34"/>
-      <c r="B20" s="32">
+      <c r="A20" s="33"/>
+      <c r="B20" s="31">
         <v>5</v>
       </c>
       <c r="C20" s="17">
@@ -13227,43 +13220,43 @@
     </row>
     <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="23.25">
       <c r="A21" s="1"/>
-      <c r="B21" s="35" t="s">
+      <c r="B21" s="34" t="s">
         <v>14</v>
       </c>
-      <c r="C21" s="36">
+      <c r="C21" s="35">
         <v>68.2</v>
       </c>
-      <c r="D21" s="36">
+      <c r="D21" s="35">
         <v>7.82</v>
       </c>
-      <c r="E21" s="36">
+      <c r="E21" s="35">
         <v>67.2</v>
       </c>
-      <c r="F21" s="36">
+      <c r="F21" s="35">
         <v>8.62</v>
       </c>
-      <c r="G21" s="36">
+      <c r="G21" s="35">
         <v>71.8</v>
       </c>
-      <c r="H21" s="36">
+      <c r="H21" s="35">
         <v>7.78</v>
       </c>
-      <c r="I21" s="37">
+      <c r="I21" s="36">
         <v>69</v>
       </c>
-      <c r="J21" s="36">
+      <c r="J21" s="35">
         <v>8.08</v>
       </c>
-      <c r="K21" s="36">
+      <c r="K21" s="35">
         <v>68.2</v>
       </c>
-      <c r="L21" s="36">
+      <c r="L21" s="35">
         <v>8.34</v>
       </c>
-      <c r="M21" s="36">
+      <c r="M21" s="35">
         <v>68.6</v>
       </c>
-      <c r="N21" s="36">
+      <c r="N21" s="35">
         <v>8.1</v>
       </c>
       <c r="O21" s="1"/>
@@ -13490,16 +13483,16 @@
       <c r="T26" s="4"/>
       <c r="U26" s="4"/>
       <c r="V26" s="4"/>
-      <c r="W26" s="30"/>
-      <c r="X26" s="30"/>
+      <c r="W26" s="29"/>
+      <c r="X26" s="29"/>
       <c r="Y26" s="29"/>
       <c r="Z26" s="29"/>
       <c r="AA26" s="29"/>
-      <c r="AB26" s="30"/>
-      <c r="AC26" s="30"/>
-      <c r="AD26" s="30"/>
-      <c r="AE26" s="30"/>
-      <c r="AF26" s="30"/>
+      <c r="AB26" s="29"/>
+      <c r="AC26" s="29"/>
+      <c r="AD26" s="29"/>
+      <c r="AE26" s="29"/>
+      <c r="AF26" s="29"/>
     </row>
     <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="28.5">
       <c r="A27" s="1"/>
@@ -13545,19 +13538,19 @@
       <c r="Q27" s="28"/>
       <c r="R27" s="28"/>
       <c r="S27" s="4"/>
-      <c r="T27" s="30"/>
-      <c r="U27" s="30"/>
+      <c r="T27" s="29"/>
+      <c r="U27" s="29"/>
       <c r="V27" s="29"/>
       <c r="W27" s="29"/>
       <c r="X27" s="29"/>
       <c r="Y27" s="29"/>
-      <c r="Z27" s="30"/>
-      <c r="AA27" s="30"/>
-      <c r="AB27" s="30"/>
-      <c r="AC27" s="30"/>
-      <c r="AD27" s="30"/>
-      <c r="AE27" s="30"/>
-      <c r="AF27" s="30"/>
+      <c r="Z27" s="29"/>
+      <c r="AA27" s="29"/>
+      <c r="AB27" s="29"/>
+      <c r="AC27" s="29"/>
+      <c r="AD27" s="29"/>
+      <c r="AE27" s="29"/>
+      <c r="AF27" s="29"/>
     </row>
     <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="18.75">
       <c r="A28" s="15" t="s">
@@ -13607,17 +13600,17 @@
       <c r="Q28" s="28"/>
       <c r="R28" s="28"/>
       <c r="S28" s="4"/>
-      <c r="T28" s="30"/>
-      <c r="U28" s="30"/>
+      <c r="T28" s="29"/>
+      <c r="U28" s="29"/>
       <c r="V28" s="29"/>
       <c r="W28" s="29"/>
       <c r="X28" s="29"/>
       <c r="Y28" s="29"/>
-      <c r="Z28" s="30"/>
-      <c r="AA28" s="30"/>
-      <c r="AB28" s="30"/>
-      <c r="AC28" s="30"/>
-      <c r="AD28" s="30"/>
+      <c r="Z28" s="29"/>
+      <c r="AA28" s="29"/>
+      <c r="AB28" s="29"/>
+      <c r="AC28" s="29"/>
+      <c r="AD28" s="29"/>
       <c r="AE28" s="4"/>
       <c r="AF28" s="4"/>
     </row>
@@ -13863,43 +13856,43 @@
     </row>
     <row x14ac:dyDescent="0.25" r="33" customHeight="1" ht="18.75">
       <c r="A33" s="1"/>
-      <c r="B33" s="35" t="s">
+      <c r="B33" s="34" t="s">
         <v>14</v>
       </c>
-      <c r="C33" s="37">
-        <v>68</v>
-      </c>
-      <c r="D33" s="36">
+      <c r="C33" s="36">
+        <v>68</v>
+      </c>
+      <c r="D33" s="35">
         <v>8.28</v>
       </c>
-      <c r="E33" s="37">
-        <v>68</v>
-      </c>
-      <c r="F33" s="36">
+      <c r="E33" s="36">
+        <v>68</v>
+      </c>
+      <c r="F33" s="35">
         <v>8.56</v>
       </c>
-      <c r="G33" s="36">
+      <c r="G33" s="35">
         <v>68.6</v>
       </c>
-      <c r="H33" s="36">
+      <c r="H33" s="35">
         <v>8.24</v>
       </c>
-      <c r="I33" s="36">
+      <c r="I33" s="35">
         <v>68.2</v>
       </c>
-      <c r="J33" s="36">
+      <c r="J33" s="35">
         <v>8.5</v>
       </c>
-      <c r="K33" s="37">
+      <c r="K33" s="36">
         <v>70</v>
       </c>
-      <c r="L33" s="36">
+      <c r="L33" s="35">
         <v>8.24</v>
       </c>
-      <c r="M33" s="36">
+      <c r="M33" s="35">
         <v>69.2</v>
       </c>
-      <c r="N33" s="36">
+      <c r="N33" s="35">
         <v>8.42</v>
       </c>
       <c r="O33" s="1"/>
@@ -14499,43 +14492,43 @@
     </row>
     <row x14ac:dyDescent="0.25" r="45" customHeight="1" ht="18.75">
       <c r="A45" s="1"/>
-      <c r="B45" s="35" t="s">
+      <c r="B45" s="34" t="s">
         <v>14</v>
       </c>
-      <c r="C45" s="36">
+      <c r="C45" s="35">
         <v>68.4</v>
       </c>
-      <c r="D45" s="36">
+      <c r="D45" s="35">
         <v>8.52</v>
       </c>
-      <c r="E45" s="36">
+      <c r="E45" s="35">
         <v>68.6</v>
       </c>
-      <c r="F45" s="36">
+      <c r="F45" s="35">
         <f>AVERAGE(F40:F44)</f>
       </c>
-      <c r="G45" s="37">
+      <c r="G45" s="36">
         <v>69</v>
       </c>
-      <c r="H45" s="36">
+      <c r="H45" s="35">
         <v>8.1</v>
       </c>
-      <c r="I45" s="36">
+      <c r="I45" s="35">
         <v>68.8</v>
       </c>
-      <c r="J45" s="36">
+      <c r="J45" s="35">
         <v>9.2</v>
       </c>
-      <c r="K45" s="36">
+      <c r="K45" s="35">
         <v>68.2</v>
       </c>
-      <c r="L45" s="36">
+      <c r="L45" s="35">
         <v>8.32</v>
       </c>
-      <c r="M45" s="36">
+      <c r="M45" s="35">
         <v>67.8</v>
       </c>
-      <c r="N45" s="36">
+      <c r="N45" s="35">
         <v>8.76</v>
       </c>
       <c r="O45" s="1"/>
@@ -14817,18 +14810,18 @@
       <c r="Q51" s="28"/>
       <c r="R51" s="28"/>
       <c r="S51" s="4"/>
-      <c r="T51" s="30"/>
-      <c r="U51" s="30"/>
+      <c r="T51" s="29"/>
+      <c r="U51" s="29"/>
       <c r="V51" s="29"/>
       <c r="W51" s="29"/>
       <c r="X51" s="29"/>
       <c r="Y51" s="29"/>
-      <c r="Z51" s="30"/>
-      <c r="AA51" s="30"/>
-      <c r="AB51" s="30"/>
-      <c r="AC51" s="30"/>
-      <c r="AD51" s="30"/>
-      <c r="AE51" s="30"/>
+      <c r="Z51" s="29"/>
+      <c r="AA51" s="29"/>
+      <c r="AB51" s="29"/>
+      <c r="AC51" s="29"/>
+      <c r="AD51" s="29"/>
+      <c r="AE51" s="29"/>
       <c r="AF51" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="52" customHeight="1" ht="18.75">
@@ -14879,18 +14872,18 @@
       <c r="Q52" s="28"/>
       <c r="R52" s="28"/>
       <c r="S52" s="4"/>
-      <c r="T52" s="30"/>
-      <c r="U52" s="30"/>
+      <c r="T52" s="29"/>
+      <c r="U52" s="29"/>
       <c r="V52" s="29"/>
       <c r="W52" s="29"/>
       <c r="X52" s="29"/>
       <c r="Y52" s="29"/>
-      <c r="Z52" s="30"/>
-      <c r="AA52" s="30"/>
-      <c r="AB52" s="30"/>
-      <c r="AC52" s="30"/>
-      <c r="AD52" s="30"/>
-      <c r="AE52" s="30"/>
+      <c r="Z52" s="29"/>
+      <c r="AA52" s="29"/>
+      <c r="AB52" s="29"/>
+      <c r="AC52" s="29"/>
+      <c r="AD52" s="29"/>
+      <c r="AE52" s="29"/>
       <c r="AF52" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="53" customHeight="1" ht="24.600000000000005">
@@ -14939,17 +14932,17 @@
       <c r="Q53" s="1"/>
       <c r="R53" s="1"/>
       <c r="S53" s="4"/>
-      <c r="T53" s="30"/>
-      <c r="U53" s="30"/>
+      <c r="T53" s="29"/>
+      <c r="U53" s="29"/>
       <c r="V53" s="29"/>
       <c r="W53" s="29"/>
       <c r="X53" s="29"/>
       <c r="Y53" s="29"/>
-      <c r="Z53" s="30"/>
-      <c r="AA53" s="30"/>
-      <c r="AB53" s="30"/>
-      <c r="AC53" s="30"/>
-      <c r="AD53" s="30"/>
+      <c r="Z53" s="29"/>
+      <c r="AA53" s="29"/>
+      <c r="AB53" s="29"/>
+      <c r="AC53" s="29"/>
+      <c r="AD53" s="29"/>
       <c r="AE53" s="4"/>
       <c r="AF53" s="4"/>
     </row>
@@ -15135,43 +15128,43 @@
     </row>
     <row x14ac:dyDescent="0.25" r="57" customHeight="1" ht="18.75">
       <c r="A57" s="1"/>
-      <c r="B57" s="35" t="s">
+      <c r="B57" s="34" t="s">
         <v>14</v>
       </c>
-      <c r="C57" s="36">
+      <c r="C57" s="35">
         <v>68.6</v>
       </c>
-      <c r="D57" s="36">
+      <c r="D57" s="35">
         <v>8.48</v>
       </c>
-      <c r="E57" s="36">
+      <c r="E57" s="35">
         <v>68.2</v>
       </c>
-      <c r="F57" s="36">
+      <c r="F57" s="35">
         <v>8.76</v>
       </c>
-      <c r="G57" s="37">
+      <c r="G57" s="36">
         <v>69</v>
       </c>
-      <c r="H57" s="36">
+      <c r="H57" s="35">
         <v>8.98</v>
       </c>
-      <c r="I57" s="36">
+      <c r="I57" s="35">
         <v>67.4</v>
       </c>
-      <c r="J57" s="36">
+      <c r="J57" s="35">
         <v>8.78</v>
       </c>
-      <c r="K57" s="36">
+      <c r="K57" s="35">
         <v>68.8</v>
       </c>
-      <c r="L57" s="36">
+      <c r="L57" s="35">
         <v>8.22</v>
       </c>
-      <c r="M57" s="36">
+      <c r="M57" s="35">
         <v>68.4</v>
       </c>
-      <c r="N57" s="36">
+      <c r="N57" s="35">
         <v>8.78</v>
       </c>
       <c r="O57" s="1"/>
@@ -15771,43 +15764,43 @@
     </row>
     <row x14ac:dyDescent="0.25" r="69" customHeight="1" ht="18.75">
       <c r="A69" s="1"/>
-      <c r="B69" s="35" t="s">
+      <c r="B69" s="34" t="s">
         <v>14</v>
       </c>
-      <c r="C69" s="36">
+      <c r="C69" s="35">
         <v>67.8</v>
       </c>
-      <c r="D69" s="36">
+      <c r="D69" s="35">
         <v>9.34</v>
       </c>
-      <c r="E69" s="36">
+      <c r="E69" s="35">
         <v>67.4</v>
       </c>
-      <c r="F69" s="36">
+      <c r="F69" s="35">
         <v>8.88</v>
       </c>
-      <c r="G69" s="37">
-        <v>68</v>
-      </c>
-      <c r="H69" s="36">
+      <c r="G69" s="36">
+        <v>68</v>
+      </c>
+      <c r="H69" s="35">
         <v>9.54</v>
       </c>
-      <c r="I69" s="36">
+      <c r="I69" s="35">
         <v>67.6</v>
       </c>
-      <c r="J69" s="36">
+      <c r="J69" s="35">
         <v>9.46</v>
       </c>
-      <c r="K69" s="37">
-        <v>68</v>
-      </c>
-      <c r="L69" s="36">
+      <c r="K69" s="36">
+        <v>68</v>
+      </c>
+      <c r="L69" s="35">
         <v>8.36</v>
       </c>
-      <c r="M69" s="36">
+      <c r="M69" s="35">
         <v>67.2</v>
       </c>
-      <c r="N69" s="36">
+      <c r="N69" s="35">
         <v>8.68</v>
       </c>
       <c r="O69" s="1"/>
@@ -16104,10 +16097,10 @@
       <c r="AF75" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="76" customHeight="1" ht="18.75">
-      <c r="A76" s="31" t="s">
+      <c r="A76" s="30" t="s">
         <v>25</v>
       </c>
-      <c r="B76" s="32">
+      <c r="B76" s="31">
         <v>1</v>
       </c>
       <c r="C76" s="17">
@@ -16166,8 +16159,8 @@
       <c r="AF76" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="77" customHeight="1" ht="18.75">
-      <c r="A77" s="33"/>
-      <c r="B77" s="32">
+      <c r="A77" s="32"/>
+      <c r="B77" s="31">
         <v>2</v>
       </c>
       <c r="C77" s="17">
@@ -16226,8 +16219,8 @@
       <c r="AF77" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="78" customHeight="1" ht="18.75">
-      <c r="A78" s="33"/>
-      <c r="B78" s="32">
+      <c r="A78" s="32"/>
+      <c r="B78" s="31">
         <v>3</v>
       </c>
       <c r="C78" s="17">
@@ -16286,8 +16279,8 @@
       <c r="AF78" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="79" customHeight="1" ht="18.75">
-      <c r="A79" s="33"/>
-      <c r="B79" s="32">
+      <c r="A79" s="32"/>
+      <c r="B79" s="31">
         <v>4</v>
       </c>
       <c r="C79" s="17">
@@ -16346,8 +16339,8 @@
       <c r="AF79" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="80" customHeight="1" ht="18.75">
-      <c r="A80" s="34"/>
-      <c r="B80" s="32">
+      <c r="A80" s="33"/>
+      <c r="B80" s="31">
         <v>5</v>
       </c>
       <c r="C80" s="17">
@@ -16407,43 +16400,43 @@
     </row>
     <row x14ac:dyDescent="0.25" r="81" customHeight="1" ht="18.75">
       <c r="A81" s="1"/>
-      <c r="B81" s="35" t="s">
+      <c r="B81" s="34" t="s">
         <v>14</v>
       </c>
-      <c r="C81" s="37">
+      <c r="C81" s="36">
         <v>67</v>
       </c>
-      <c r="D81" s="36">
+      <c r="D81" s="35">
         <v>9.38</v>
       </c>
-      <c r="E81" s="36">
+      <c r="E81" s="35">
         <v>66.6</v>
       </c>
-      <c r="F81" s="36">
+      <c r="F81" s="35">
         <v>9.22</v>
       </c>
-      <c r="G81" s="36">
+      <c r="G81" s="35">
         <v>67.2</v>
       </c>
-      <c r="H81" s="36">
+      <c r="H81" s="35">
         <v>8.68</v>
       </c>
-      <c r="I81" s="36">
+      <c r="I81" s="35">
         <v>67.4</v>
       </c>
-      <c r="J81" s="36">
+      <c r="J81" s="35">
         <v>8.98</v>
       </c>
-      <c r="K81" s="36">
+      <c r="K81" s="35">
         <v>67.6</v>
       </c>
-      <c r="L81" s="36">
+      <c r="L81" s="35">
         <v>8.88</v>
       </c>
-      <c r="M81" s="36">
+      <c r="M81" s="35">
         <v>67.2</v>
       </c>
-      <c r="N81" s="36">
+      <c r="N81" s="35">
         <v>8.94</v>
       </c>
       <c r="O81" s="4"/>

</xml_diff>